<commit_message>
add stock to vip
</commit_message>
<xml_diff>
--- a/stock_vip.xlsx
+++ b/stock_vip.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28140" windowHeight="16060" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28140" windowHeight="16060" tabRatio="1000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="美的集团" sheetId="21" r:id="rId1"/>
     <sheet name="贵州茅台" sheetId="24" r:id="rId2"/>
     <sheet name="东阿阿胶" sheetId="25" r:id="rId3"/>
     <sheet name="云南白药" sheetId="26" r:id="rId4"/>
+    <sheet name="中国石化" sheetId="27" r:id="rId5"/>
+    <sheet name="宝钢股份" sheetId="28" r:id="rId6"/>
+    <sheet name="华大基因" sheetId="30" r:id="rId7"/>
+    <sheet name="比亚迪" sheetId="31" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>万元</t>
   </si>
@@ -67,6 +71,18 @@
   </si>
   <si>
     <t>大户累计</t>
+  </si>
+  <si>
+    <t>中国石化</t>
+  </si>
+  <si>
+    <t>宝钢股份</t>
+  </si>
+  <si>
+    <t>华大基因</t>
+  </si>
+  <si>
+    <t>比亚迪</t>
   </si>
 </sst>
 </file>
@@ -602,10 +618,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$9:$S$9</c:f>
+              <c:f>美的集团!$D$9:$AF$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>58.14</c:v>
                 </c:pt>
@@ -653,6 +669,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>61.41</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,6 +742,894 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>中国石化!$D$11:$AP$11</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-973.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>中国石化!$D$12:$AP$12</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>4267.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>中国石化!$D$13:$AP$13</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-5241.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2143780920"/>
+        <c:axId val="-2144160584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2143780920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2144160584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2144160584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[Red]0.00;[Green]\-0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2143780920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>宝钢股份!$D$9:$AN$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>9.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1992148632"/>
+        <c:axId val="2128484360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1992148632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128484360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2128484360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00;[Red]#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1992148632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>宝钢股份!$D$11:$AP$11</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-2801.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>宝钢股份!$D$12:$AP$12</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>178.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>宝钢股份!$D$13:$AP$13</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-2979.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2128431800"/>
+        <c:axId val="-2088335512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2128431800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2088335512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2088335512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[Red]0.00;[Green]\-0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128431800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>华大基因!$D$9:$AN$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>166.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1999927832"/>
+        <c:axId val="-2144152440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1999927832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2144152440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2144152440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00;[Red]#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1999927832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>华大基因!$D$11:$AP$11</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-760.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>华大基因!$D$12:$AP$12</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-1391.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>华大基因!$D$13:$AP$13</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>631.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1993837400"/>
+        <c:axId val="-1993834424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1993837400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1993834424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1993834424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[Red]0.00;[Green]\-0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1993837400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>比亚迪!$D$9:$AN$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>166.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1999862456"/>
+        <c:axId val="-1999859784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1999862456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1999859784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1999859784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00;[Red]#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1999862456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>比亚迪!$D$11:$AP$11</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-1264.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>比亚迪!$D$12:$AP$12</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-842.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>比亚迪!$D$13:$AP$13</c:f>
+              <c:numCache>
+                <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>-421.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2080060072"/>
+        <c:axId val="-2113527368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2080060072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2113527368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2113527368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[Red]0.00;[Green]\-0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2080060072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -751,10 +1658,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$11:$S$11</c:f>
+              <c:f>美的集团!$D$11:$AD$11</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>4399.61</c:v>
                 </c:pt>
@@ -802,6 +1709,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>30533.91000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19037.18000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -816,10 +1726,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$12:$S$12</c:f>
+              <c:f>美的集团!$D$12:$AD$12</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>9844.74</c:v>
                 </c:pt>
@@ -867,6 +1777,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>90988.74</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>78601.41999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -881,10 +1794,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$13:$S$13</c:f>
+              <c:f>美的集团!$D$13:$AD$13</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>-5445.13</c:v>
                 </c:pt>
@@ -932,6 +1845,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-60453.79000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-59563.21000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1030,10 +1946,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>贵州茅台!$D$9:$S$9</c:f>
+              <c:f>贵州茅台!$D$9:$AL$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>742.45</c:v>
                 </c:pt>
@@ -1081,6 +1997,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>746.47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>739.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1179,10 +2098,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>贵州茅台!$D$11:$S$11</c:f>
+              <c:f>贵州茅台!$D$11:$AK$11</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>72.31</c:v>
                 </c:pt>
@@ -1230,6 +2149,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2624.28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2699.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,10 +2166,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>贵州茅台!$D$12:$S$12</c:f>
+              <c:f>贵州茅台!$D$12:$AK$12</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>21295.58</c:v>
                 </c:pt>
@@ -1295,6 +2217,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-10188.66</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2450.020000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,10 +2234,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>贵州茅台!$D$13:$S$13</c:f>
+              <c:f>贵州茅台!$D$13:$AK$13</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>-21223.27</c:v>
                 </c:pt>
@@ -1360,6 +2285,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>12812.88999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5149.519999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1458,10 +2386,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>东阿阿胶!$D$9:$S$9</c:f>
+              <c:f>东阿阿胶!$D$9:$AD$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>62.55</c:v>
                 </c:pt>
@@ -1509,6 +2437,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>60.74</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>61.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1607,10 +2538,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>东阿阿胶!$D$11:$S$11</c:f>
+              <c:f>东阿阿胶!$D$11:$AG$11</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-1885.61</c:v>
                 </c:pt>
@@ -1658,6 +2589,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-7276.300000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-5980.570000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1672,10 +2606,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>东阿阿胶!$D$12:$S$12</c:f>
+              <c:f>东阿阿胶!$D$12:$AG$12</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-2086.26</c:v>
                 </c:pt>
@@ -1723,6 +2657,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-22068.77</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-19592.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,10 +2674,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>东阿阿胶!$D$13:$S$13</c:f>
+              <c:f>东阿阿胶!$D$13:$AG$13</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>200.65</c:v>
                 </c:pt>
@@ -1788,6 +2725,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>14792.48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13612.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1886,10 +2826,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>云南白药!$D$9:$S$9</c:f>
+              <c:f>云南白药!$D$9:$AN$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>96.2</c:v>
                 </c:pt>
@@ -1937,6 +2877,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>101.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2035,10 +2978,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>云南白药!$D$11:$S$11</c:f>
+              <c:f>云南白药!$D$11:$AP$11</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>2500.3</c:v>
                 </c:pt>
@@ -2086,6 +3029,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>6498.910000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6601.950000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2100,10 +3046,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>云南白药!$D$12:$S$12</c:f>
+              <c:f>云南白药!$D$12:$AP$12</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>3192.81</c:v>
                 </c:pt>
@@ -2151,6 +3097,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>13207.76</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13463.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2165,10 +3114,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>云南白药!$D$13:$S$13</c:f>
+              <c:f>云南白药!$D$13:$AP$13</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>-692.51</c:v>
                 </c:pt>
@@ -2216,6 +3165,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>-6738.84</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6891.869999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2286,6 +3238,110 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>中国石化!$D$9:$AN$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>6.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2131858776"/>
+        <c:axId val="2116651688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2131858776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2116651688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2116651688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00;[Red]#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2131858776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2326,10 +3382,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2355,16 +3411,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2391,8 +3447,8 @@
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -2426,10 +3482,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2456,10 +3512,10 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>679450</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2491,10 +3547,10 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2516,20 +3572,296 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>679450</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2870,8 +4202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4725,7 +6057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
@@ -5651,7 +6983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
@@ -6571,4 +7903,2340 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>955.58</v>
+      </c>
+      <c r="F2">
+        <f>E2*10000</f>
+        <v>9555800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6">
+        <v>8</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>11</v>
+      </c>
+      <c r="O4" s="6">
+        <v>12</v>
+      </c>
+      <c r="P4" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>14</v>
+      </c>
+      <c r="R4" s="6">
+        <v>15</v>
+      </c>
+      <c r="S4" s="6">
+        <v>16</v>
+      </c>
+      <c r="T4" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43175</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43178</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43179</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43180</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43181</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43182</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="6"/>
+      <c r="B6" s="12">
+        <f>SUM(D6:IX6)</f>
+        <v>-973.91</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-973.91</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="6"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4267.2299999999996</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-5241.1400000000003</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>6.42</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <f>B10/F2</f>
+        <v>-1.5875110084664864E-5</v>
+      </c>
+      <c r="B10" s="3">
+        <f>SUM(D10:IX10)</f>
+        <v>-151.69937694704049</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ref="D10:T10" si="0">D6/D9</f>
+        <v>-151.69937694704049</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-973.91</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>4267.2299999999996</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-5241.1400000000003</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6">
+        <f>B6/B10</f>
+        <v>6.42</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="8"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>220.9</v>
+      </c>
+      <c r="F2">
+        <f>E2*10000</f>
+        <v>2209000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6">
+        <v>8</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>11</v>
+      </c>
+      <c r="O4" s="6">
+        <v>12</v>
+      </c>
+      <c r="P4" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>14</v>
+      </c>
+      <c r="R4" s="6">
+        <v>15</v>
+      </c>
+      <c r="S4" s="6">
+        <v>16</v>
+      </c>
+      <c r="T4" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43175</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43178</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43179</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43180</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43181</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43182</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="6"/>
+      <c r="B6" s="12">
+        <f>SUM(D6:IX6)</f>
+        <v>-2801.16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-2801.16</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="6"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>178.46</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-2979.62</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>9.41</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <f>B10/F2</f>
+        <v>-1.3475738561550686E-4</v>
+      </c>
+      <c r="B10" s="3">
+        <f>SUM(D10:IX10)</f>
+        <v>-297.67906482465463</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ref="D10:T10" si="0">D6/D9</f>
+        <v>-297.67906482465463</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-2801.16</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>178.46</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-2979.62</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6">
+        <f>B6/B10</f>
+        <v>9.4099999999999984</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="8"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="F2">
+        <f>E2*10000</f>
+        <v>4010.0000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6">
+        <v>8</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>11</v>
+      </c>
+      <c r="O4" s="6">
+        <v>12</v>
+      </c>
+      <c r="P4" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>14</v>
+      </c>
+      <c r="R4" s="6">
+        <v>15</v>
+      </c>
+      <c r="S4" s="6">
+        <v>16</v>
+      </c>
+      <c r="T4" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43175</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43178</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43179</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43180</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43181</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43182</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="6"/>
+      <c r="B6" s="12">
+        <f>SUM(D6:IX6)</f>
+        <v>-760.11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-760.11</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="6"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-1391.2</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>631.09</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>166.22</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <f>B10/F2</f>
+        <v>-1.1403779085555272E-3</v>
+      </c>
+      <c r="B10" s="3">
+        <f>SUM(D10:IX10)</f>
+        <v>-4.5729154133076646</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ref="D10:T10" si="0">D6/D9</f>
+        <v>-4.5729154133076646</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-760.11</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-1391.2</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>631.09</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6">
+        <f>B6/B10</f>
+        <v>166.22</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="8"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>11.38</v>
+      </c>
+      <c r="F2">
+        <f>E2*10000</f>
+        <v>113800.00000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6">
+        <v>8</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6">
+        <v>11</v>
+      </c>
+      <c r="O4" s="6">
+        <v>12</v>
+      </c>
+      <c r="P4" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>14</v>
+      </c>
+      <c r="R4" s="6">
+        <v>15</v>
+      </c>
+      <c r="S4" s="6">
+        <v>16</v>
+      </c>
+      <c r="T4" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43175</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43178</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43179</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43180</v>
+      </c>
+      <c r="H5" s="5">
+        <v>43181</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43182</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="6"/>
+      <c r="B6" s="12">
+        <f>SUM(D6:IX6)</f>
+        <v>-1264.26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-1264.26</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="6"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-842.29</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-421.96</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>166.22</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <f>B10/F2</f>
+        <v>-6.6836062651420735E-5</v>
+      </c>
+      <c r="B10" s="3">
+        <f>SUM(D10:IX10)</f>
+        <v>-7.6059439297316809</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ref="D10:T10" si="0">D6/D9</f>
+        <v>-7.6059439297316809</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-1264.26</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-842.29</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-421.96</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6">
+        <f>B6/B10</f>
+        <v>166.22</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="8"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adjust range of data
</commit_message>
<xml_diff>
--- a/stock_vip.xlsx
+++ b/stock_vip.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28140" windowHeight="16060" tabRatio="1000" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28140" windowHeight="16060" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="美的集团" sheetId="21" r:id="rId1"/>
@@ -630,10 +630,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$9:$AF$9</c:f>
+              <c:f>美的集团!$D$9:$CF$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;[Red]#,##0.00</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>58.14</c:v>
                 </c:pt>
@@ -775,6 +775,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2245,10 +2246,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$11:$AD$11</c:f>
+              <c:f>美的集团!$D$11:$CD$11</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>4399.61</c:v>
                 </c:pt>
@@ -2329,6 +2330,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>-34166.72</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-48449.55</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-47273.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2343,10 +2350,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$12:$AD$12</c:f>
+              <c:f>美的集团!$D$12:$CD$12</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>9844.74</c:v>
                 </c:pt>
@@ -2427,6 +2434,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>51925.69999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40628.00999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>48606.91999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2441,10 +2454,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>美的集团!$D$13:$AD$13</c:f>
+              <c:f>美的集团!$D$13:$CD$13</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-5445.13</c:v>
                 </c:pt>
@@ -2525,6 +2538,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>-86091.33</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-89076.41</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-95879.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2580,6 +2599,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2767,6 +2787,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3162,6 +3183,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3343,6 +3365,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3738,6 +3761,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4479,16 +4503,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1060450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4510,15 +4534,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1212850</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>1060450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5335,7 +5359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
@@ -6672,7 +6696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
@@ -8006,7 +8030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
@@ -13188,7 +13212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
2018-5-25 ~ 2018-5-30 update
</commit_message>
<xml_diff>
--- a/stock_vip.xlsx
+++ b/stock_vip.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="1000" activeTab="7"/>
+    <workbookView xWindow="2700" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="1000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="美的集团" sheetId="21" r:id="rId1"/>
@@ -171,8 +171,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="219">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,7 +420,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="219">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -526,6 +530,8 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -635,6 +641,8 @@
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,6 +878,18 @@
                 <c:pt idx="61">
                   <c:v>50.9</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>50.59</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>51.94</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>51.49</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>50.71</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -885,11 +905,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1988811512"/>
-        <c:axId val="-2074186552"/>
+        <c:axId val="2081511208"/>
+        <c:axId val="2081981032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1988811512"/>
+        <c:axId val="2081511208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074186552"/>
+        <c:crossAx val="2081981032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -906,7 +926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074186552"/>
+        <c:axId val="2081981032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45.0"/>
@@ -918,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1988811512"/>
+        <c:crossAx val="2081511208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1105,6 +1125,18 @@
                 <c:pt idx="45">
                   <c:v>3469.020000000016</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-3377.019999999984</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-6772.619999999984</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-5748.229999999984</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-9860.649999999983</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1260,6 +1292,18 @@
                 <c:pt idx="45">
                   <c:v>86152.15</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>75585.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>73615.26999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>70811.48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>66575.26999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1415,6 +1459,18 @@
                 <c:pt idx="45">
                   <c:v>-82757.05000000001</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-79036.33000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-80461.79000000002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-76633.60000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-76509.81000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1430,11 +1486,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074323880"/>
-        <c:axId val="-2074327400"/>
+        <c:axId val="2081998168"/>
+        <c:axId val="2104678232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074323880"/>
+        <c:axId val="2081998168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,7 +1499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074327400"/>
+        <c:crossAx val="2104678232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1451,7 +1507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074327400"/>
+        <c:axId val="2104678232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,7 +1518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074323880"/>
+        <c:crossAx val="2081998168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1649,6 +1705,18 @@
                 <c:pt idx="45">
                   <c:v>8.46</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.42</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.57</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1664,11 +1732,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1887907352"/>
-        <c:axId val="1887900824"/>
+        <c:axId val="2082171944"/>
+        <c:axId val="2046902648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1887907352"/>
+        <c:axId val="2082171944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,7 +1745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1887900824"/>
+        <c:crossAx val="2046902648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1685,7 +1753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1887900824"/>
+        <c:axId val="2046902648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1764,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1887907352"/>
+        <c:crossAx val="2082171944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1883,6 +1951,18 @@
                 <c:pt idx="45">
                   <c:v>-84993.88</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-89170.28</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-90404.13</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-83721.74000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-89667.55</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2038,6 +2118,18 @@
                 <c:pt idx="45">
                   <c:v>-44359.45999999998</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-46307.76999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-50341.23999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-41661.49999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-48662.07999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2193,6 +2285,18 @@
                 <c:pt idx="45">
                   <c:v>-41741.87</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-43969.96</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-41170.33999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-43167.69999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-42112.92</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2208,11 +2312,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074443640"/>
-        <c:axId val="-2074448088"/>
+        <c:axId val="2082232376"/>
+        <c:axId val="2105408760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074443640"/>
+        <c:axId val="2082232376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074448088"/>
+        <c:crossAx val="2105408760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2229,7 +2333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074448088"/>
+        <c:axId val="2105408760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,7 +2344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074443640"/>
+        <c:crossAx val="2082232376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2427,6 +2531,18 @@
                 <c:pt idx="45">
                   <c:v>152.26</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>148.72</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>147.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>145.97</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>137.13</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2442,11 +2558,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1887811672"/>
-        <c:axId val="1887814728"/>
+        <c:axId val="2082234104"/>
+        <c:axId val="2104883096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1887811672"/>
+        <c:axId val="2082234104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2455,7 +2571,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1887814728"/>
+        <c:crossAx val="2104883096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2463,7 +2579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1887814728"/>
+        <c:axId val="2104883096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="130.0"/>
@@ -2475,7 +2591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1887811672"/>
+        <c:crossAx val="2082234104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2662,6 +2778,18 @@
                 <c:pt idx="45">
                   <c:v>-50425.09</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-53324.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-54207.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-55343.01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-58578.47</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2817,6 +2945,18 @@
                 <c:pt idx="45">
                   <c:v>-28594.01</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-30068.38</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-30915.51</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-31108.27</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-32888.14</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2972,6 +3112,18 @@
                 <c:pt idx="45">
                   <c:v>-20565.06</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-21990.09</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-22025.93</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-22968.71</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-24424.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2987,11 +3139,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1974780632"/>
-        <c:axId val="-1974777656"/>
+        <c:axId val="2105125800"/>
+        <c:axId val="2046980392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1974780632"/>
+        <c:axId val="2105125800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,7 +3152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1974777656"/>
+        <c:crossAx val="2046980392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3008,7 +3160,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1974777656"/>
+        <c:axId val="2046980392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3019,7 +3171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1974780632"/>
+        <c:crossAx val="2105125800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3206,6 +3358,18 @@
                 <c:pt idx="45">
                   <c:v>54.15</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>54.22</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>52.78</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3221,11 +3385,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074628040"/>
-        <c:axId val="-2074659272"/>
+        <c:axId val="2082446472"/>
+        <c:axId val="2048106104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074628040"/>
+        <c:axId val="2082446472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3234,7 +3398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074659272"/>
+        <c:crossAx val="2048106104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3242,7 +3406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074659272"/>
+        <c:axId val="2048106104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45.0"/>
@@ -3254,7 +3418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074628040"/>
+        <c:crossAx val="2082446472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3441,6 +3605,18 @@
                 <c:pt idx="45">
                   <c:v>-122336.52</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-122765.47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-126721.53</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-128652.14</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-135147.52</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3596,6 +3772,18 @@
                 <c:pt idx="45">
                   <c:v>-143822.74</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>-145343.0900000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-148326.2200000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-150664.6500000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-154049.73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3751,6 +3939,18 @@
                 <c:pt idx="45">
                   <c:v>28306.98999999999</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>29398.38999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>28425.45999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>28833.26999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>25722.97999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3766,11 +3966,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074847720"/>
-        <c:axId val="-2074848808"/>
+        <c:axId val="2104600296"/>
+        <c:axId val="2105268312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074847720"/>
+        <c:axId val="2104600296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,7 +3979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074848808"/>
+        <c:crossAx val="2105268312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3787,7 +3987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074848808"/>
+        <c:axId val="2105268312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3798,7 +3998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074847720"/>
+        <c:crossAx val="2104600296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4033,6 +4233,18 @@
                 <c:pt idx="61">
                   <c:v>-184547.87</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-194286.02</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-191512.87</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-192936.94</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-197640.66</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4236,6 +4448,18 @@
                 <c:pt idx="61">
                   <c:v>-53231.56000000002</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-57946.52000000002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-50587.60000000002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-48483.59000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-51520.22000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4439,6 +4663,18 @@
                 <c:pt idx="61">
                   <c:v>-131315.38</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-136338.58</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-140924.38</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-144452.46</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-146119.58</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4454,11 +4690,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1974713016"/>
-        <c:axId val="-1974717448"/>
+        <c:axId val="2047266728"/>
+        <c:axId val="2105444024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1974713016"/>
+        <c:axId val="2047266728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4467,7 +4703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1974717448"/>
+        <c:crossAx val="2105444024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4475,7 +4711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1974717448"/>
+        <c:axId val="2105444024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4486,7 +4722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1974713016"/>
+        <c:crossAx val="2047266728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4721,6 +4957,18 @@
                 <c:pt idx="61">
                   <c:v>715.4</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>716.86</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>740.4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>731.4299999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>725.87</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4736,11 +4984,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074223176"/>
-        <c:axId val="-2074234392"/>
+        <c:axId val="2105034136"/>
+        <c:axId val="2081492392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074223176"/>
+        <c:axId val="2105034136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4749,7 +4997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074234392"/>
+        <c:crossAx val="2081492392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4757,7 +5005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074234392"/>
+        <c:axId val="2081492392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4768,7 +5016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074223176"/>
+        <c:crossAx val="2105034136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5003,6 +5251,18 @@
                 <c:pt idx="61">
                   <c:v>10279.56</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>10351.69</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>11219.72</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>11553.96</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>12485.82</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5206,6 +5466,18 @@
                 <c:pt idx="61">
                   <c:v>-83049.31</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-98002.63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-82160.66</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-69383.09</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-77061.21</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5409,6 +5681,18 @@
                 <c:pt idx="61">
                   <c:v>93329.13</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>108354.67</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>93380.77000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>80937.43000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>89547.30000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5424,11 +5708,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074293832"/>
-        <c:axId val="-2074299688"/>
+        <c:axId val="2081667912"/>
+        <c:axId val="2047964664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074293832"/>
+        <c:axId val="2081667912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5437,7 +5721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074299688"/>
+        <c:crossAx val="2047964664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5445,7 +5729,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074299688"/>
+        <c:axId val="2047964664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5456,7 +5740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074293832"/>
+        <c:crossAx val="2081667912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5691,6 +5975,18 @@
                 <c:pt idx="61">
                   <c:v>56.79</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>56.29</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>57.65</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>57.54</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>57.92</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5706,11 +6002,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1888012600"/>
-        <c:axId val="1888015656"/>
+        <c:axId val="2104985016"/>
+        <c:axId val="2081798936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1888012600"/>
+        <c:axId val="2104985016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5719,7 +6015,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888015656"/>
+        <c:crossAx val="2081798936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5727,7 +6023,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1888015656"/>
+        <c:axId val="2081798936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="47.0"/>
@@ -5739,7 +6035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888012600"/>
+        <c:crossAx val="2104985016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5974,6 +6270,18 @@
                 <c:pt idx="61">
                   <c:v>-90662.51000000002</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-91623.86000000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-89735.83000000003</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-87893.98000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-86128.91000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6177,6 +6485,18 @@
                 <c:pt idx="61">
                   <c:v>-72263.81999999997</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-75535.66999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-75890.70999999997</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-74684.04999999997</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-76535.03999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6380,6 +6700,18 @@
                 <c:pt idx="61">
                   <c:v>-18398.73</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-16088.24</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-13845.18</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-13209.99</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-9593.919999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6395,11 +6727,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1888060280"/>
-        <c:axId val="1888063256"/>
+        <c:axId val="2081992760"/>
+        <c:axId val="2081989752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1888060280"/>
+        <c:axId val="2081992760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6408,7 +6740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888063256"/>
+        <c:crossAx val="2081989752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6416,7 +6748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1888063256"/>
+        <c:axId val="2081989752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6427,7 +6759,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888060280"/>
+        <c:crossAx val="2081992760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6662,6 +6994,18 @@
                 <c:pt idx="61">
                   <c:v>116.11</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>116.96</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>118.45</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>110.03</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>108.27</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6677,11 +7021,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1888105128"/>
-        <c:axId val="1888108136"/>
+        <c:axId val="2046936264"/>
+        <c:axId val="2105511832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1888105128"/>
+        <c:axId val="2046936264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6690,7 +7034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888108136"/>
+        <c:crossAx val="2105511832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6698,7 +7042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1888108136"/>
+        <c:axId val="2105511832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6709,7 +7053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888105128"/>
+        <c:crossAx val="2046936264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6944,6 +7288,18 @@
                 <c:pt idx="61">
                   <c:v>-3011.81</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-2815.9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-4446.940000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-8521.24</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-11178.28</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7147,6 +7503,18 @@
                 <c:pt idx="61">
                   <c:v>12624.07</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>12340.87</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>10340.84999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6864.129999999995</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6050.009999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7350,6 +7718,18 @@
                 <c:pt idx="61">
                   <c:v>-15667.59999999998</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>-15188.48999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-14819.50999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-15417.11999999998</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-17260.04999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7365,11 +7745,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1995629192"/>
-        <c:axId val="-1995626216"/>
+        <c:axId val="2047180888"/>
+        <c:axId val="2081700632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1995629192"/>
+        <c:axId val="2047180888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7378,7 +7758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1995626216"/>
+        <c:crossAx val="2081700632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7386,7 +7766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1995626216"/>
+        <c:axId val="2081700632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7397,7 +7777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1995629192"/>
+        <c:crossAx val="2047180888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7584,6 +7964,18 @@
                 <c:pt idx="45">
                   <c:v>7.0</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.96</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.92</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.95</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.83</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7599,11 +7991,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1995651544"/>
-        <c:axId val="-1995658424"/>
+        <c:axId val="2104760008"/>
+        <c:axId val="2105522472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1995651544"/>
+        <c:axId val="2104760008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7612,7 +8004,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1995658424"/>
+        <c:crossAx val="2105522472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7620,7 +8012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1995658424"/>
+        <c:axId val="2105522472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7631,7 +8023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1995651544"/>
+        <c:crossAx val="2104760008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8506,10 +8898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM49"/>
+  <dimension ref="A1:BQ49"/>
   <sheetViews>
     <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BM7" sqref="BM7"/>
+      <selection activeCell="BQ7" sqref="BQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8518,7 +8910,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:69">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -8526,7 +8918,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:69">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8" t="s">
@@ -8543,7 +8935,7 @@
         <v>630800</v>
       </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:69">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="8" t="s">
@@ -8553,7 +8945,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:69">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -8743,8 +9135,20 @@
       <c r="BM4" s="6">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:65">
+      <c r="BN4" s="6">
+        <v>63</v>
+      </c>
+      <c r="BO4" s="6">
+        <v>64</v>
+      </c>
+      <c r="BP4" s="6">
+        <v>65</v>
+      </c>
+      <c r="BQ4" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -8936,12 +9340,24 @@
       <c r="BM5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:65">
+      <c r="BN5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="BO5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="BP5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BQ5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-184547.87</v>
+        <v>-197640.66</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -9132,8 +9548,20 @@
       <c r="BM6" s="2">
         <v>-12936.18</v>
       </c>
-    </row>
-    <row r="7" spans="1:65">
+      <c r="BN6" s="2">
+        <v>-9738.15</v>
+      </c>
+      <c r="BO6" s="2">
+        <v>2773.15</v>
+      </c>
+      <c r="BP6" s="2">
+        <v>-1424.07</v>
+      </c>
+      <c r="BQ6" s="2">
+        <v>-4703.72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -9325,8 +9753,20 @@
       <c r="BM7" s="2">
         <v>-10006.969999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:65">
+      <c r="BN7" s="2">
+        <v>-4714.96</v>
+      </c>
+      <c r="BO7" s="2">
+        <v>7358.92</v>
+      </c>
+      <c r="BP7" s="2">
+        <v>2104.0100000000002</v>
+      </c>
+      <c r="BQ7" s="2">
+        <v>-3036.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -9518,8 +9958,20 @@
       <c r="BM8" s="2">
         <v>-2929.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:65">
+      <c r="BN8" s="2">
+        <v>-5023.2</v>
+      </c>
+      <c r="BO8" s="2">
+        <v>-4585.8</v>
+      </c>
+      <c r="BP8" s="2">
+        <v>-3528.08</v>
+      </c>
+      <c r="BQ8" s="2">
+        <v>-1667.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -9711,15 +10163,27 @@
       <c r="BM9" s="13">
         <v>50.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:65">
+      <c r="BN9" s="13">
+        <v>50.59</v>
+      </c>
+      <c r="BO9" s="13">
+        <v>51.94</v>
+      </c>
+      <c r="BP9" s="13">
+        <v>51.49</v>
+      </c>
+      <c r="BQ9" s="13">
+        <v>50.71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-5.6658352104084391E-3</v>
+        <v>-6.0772408033788385E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-3574.0088507256432</v>
+        <v>-3833.5234987713711</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -9972,8 +10436,24 @@
         <f>BM6/BM9</f>
         <v>-254.14891944990177</v>
       </c>
-    </row>
-    <row r="11" spans="1:65">
+      <c r="BN10" s="6">
+        <f>BN6/BN9</f>
+        <v>-192.49159913026287</v>
+      </c>
+      <c r="BO10" s="6">
+        <f>BO6/BO9</f>
+        <v>53.391413169041208</v>
+      </c>
+      <c r="BP10" s="6">
+        <f>BP6/BP9</f>
+        <v>-27.657214993202562</v>
+      </c>
+      <c r="BQ10" s="6">
+        <f>BQ6/BQ9</f>
+        <v>-92.757247091303498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -10227,8 +10707,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-184547.87</v>
       </c>
-    </row>
-    <row r="12" spans="1:65">
+      <c r="BN11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-194286.02</v>
+      </c>
+      <c r="BO11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-191512.87</v>
+      </c>
+      <c r="BP11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-192936.94</v>
+      </c>
+      <c r="BQ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-197640.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -10482,8 +10978,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-53231.560000000019</v>
       </c>
-    </row>
-    <row r="13" spans="1:65">
+      <c r="BN12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-57946.520000000019</v>
+      </c>
+      <c r="BO12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-50587.60000000002</v>
+      </c>
+      <c r="BP12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-48483.590000000018</v>
+      </c>
+      <c r="BQ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-51520.220000000016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -10737,19 +11249,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-131315.38</v>
       </c>
-    </row>
-    <row r="14" spans="1:65">
+      <c r="BN13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-136338.58000000002</v>
+      </c>
+      <c r="BO13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-140924.38</v>
+      </c>
+      <c r="BP13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-144452.46</v>
+      </c>
+      <c r="BQ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-146119.57999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>51.636097644954241</v>
+        <v>51.555875440268736</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:69">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -10757,7 +11285,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:69">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -10965,10 +11493,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM49"/>
+  <dimension ref="A1:BQ49"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BM7" sqref="BM7"/>
+    <sheetView topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BQ7" sqref="BQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10977,7 +11505,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:69">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -10985,7 +11513,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:69">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -11002,14 +11530,14 @@
         <v>125600</v>
       </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:69">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:69">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -11199,8 +11727,20 @@
       <c r="BM4" s="6">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:65">
+      <c r="BN4" s="6">
+        <v>63</v>
+      </c>
+      <c r="BO4" s="6">
+        <v>64</v>
+      </c>
+      <c r="BP4" s="6">
+        <v>65</v>
+      </c>
+      <c r="BQ4" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -11392,12 +11932,24 @@
       <c r="BM5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:65">
+      <c r="BN5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="BO5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="BP5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BQ5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>10279.560000000001</v>
+        <v>12485.820000000002</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -11588,8 +12140,20 @@
       <c r="BM6" s="2">
         <v>99.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:65">
+      <c r="BN6" s="2">
+        <v>72.13</v>
+      </c>
+      <c r="BO6" s="2">
+        <v>868.03</v>
+      </c>
+      <c r="BP6" s="2">
+        <v>334.24</v>
+      </c>
+      <c r="BQ6" s="2">
+        <v>931.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -11781,8 +12345,20 @@
       <c r="BM7" s="2">
         <v>-28708.22</v>
       </c>
-    </row>
-    <row r="8" spans="1:65">
+      <c r="BN7" s="2">
+        <v>-14953.32</v>
+      </c>
+      <c r="BO7" s="2">
+        <v>15841.97</v>
+      </c>
+      <c r="BP7" s="2">
+        <v>12777.57</v>
+      </c>
+      <c r="BQ7" s="2">
+        <v>-7678.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -11974,8 +12550,20 @@
       <c r="BM8" s="2">
         <v>28808.07</v>
       </c>
-    </row>
-    <row r="9" spans="1:65">
+      <c r="BN8" s="2">
+        <v>15025.54</v>
+      </c>
+      <c r="BO8" s="2">
+        <v>-14973.9</v>
+      </c>
+      <c r="BP8" s="2">
+        <v>-12443.34</v>
+      </c>
+      <c r="BQ8" s="2">
+        <v>8609.8700000000008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -12167,15 +12755,27 @@
       <c r="BM9" s="13">
         <v>715.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:65" s="9" customFormat="1">
+      <c r="BN9" s="13">
+        <v>716.86</v>
+      </c>
+      <c r="BO9" s="13">
+        <v>740.4</v>
+      </c>
+      <c r="BP9" s="13">
+        <v>731.43</v>
+      </c>
+      <c r="BQ9" s="13">
+        <v>725.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" s="9" customFormat="1">
       <c r="A10" s="19">
         <f>B10/F2</f>
-        <v>1.1783848052666805E-4</v>
+        <v>1.418333102846503E-4</v>
       </c>
       <c r="B10" s="20">
         <f>SUM(D10:IX10)</f>
-        <v>14.800513154149508</v>
+        <v>17.814263771752078</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>3</v>
@@ -12425,11 +13025,27 @@
         <v>-2.8392605487855428E-2</v>
       </c>
       <c r="BM10" s="18">
-        <f t="shared" ref="BM10" si="28">BM6/BM9</f>
+        <f t="shared" ref="BM10:BN10" si="28">BM6/BM9</f>
         <v>0.13943248532289629</v>
       </c>
-    </row>
-    <row r="11" spans="1:65">
+      <c r="BN10" s="18">
+        <f t="shared" si="28"/>
+        <v>0.10061936779845436</v>
+      </c>
+      <c r="BO10" s="18">
+        <f t="shared" ref="BO10:BP10" si="29">BO6/BO9</f>
+        <v>1.1723797947055645</v>
+      </c>
+      <c r="BP10" s="18">
+        <f t="shared" si="29"/>
+        <v>0.45696785748465341</v>
+      </c>
+      <c r="BQ10" s="18">
+        <f t="shared" ref="BQ10" si="30">BQ6/BQ9</f>
+        <v>1.2837835976138978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -12683,8 +13299,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>10279.560000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:65">
+      <c r="BN11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>10351.69</v>
+      </c>
+      <c r="BO11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>11219.720000000001</v>
+      </c>
+      <c r="BP11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>11553.960000000001</v>
+      </c>
+      <c r="BQ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>12485.820000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -12938,8 +13570,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-83049.31</v>
       </c>
-    </row>
-    <row r="13" spans="1:65">
+      <c r="BN12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-98002.63</v>
+      </c>
+      <c r="BO12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-82160.66</v>
+      </c>
+      <c r="BP12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-69383.09</v>
+      </c>
+      <c r="BQ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-77061.209999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -13193,19 +13841,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>93329.13</v>
       </c>
-    </row>
-    <row r="14" spans="1:65">
+      <c r="BN13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>108354.67000000001</v>
+      </c>
+      <c r="BO13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>93380.770000000019</v>
+      </c>
+      <c r="BP13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>80937.430000000022</v>
+      </c>
+      <c r="BQ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>89547.300000000017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>694.54078334560984</v>
+        <v>700.88891463472419</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:69">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -13213,7 +13877,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:69">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -13421,10 +14085,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM49"/>
+  <dimension ref="A1:BQ49"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BM7" sqref="BM7"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BQ6" sqref="BQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13433,7 +14097,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:69">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -13441,7 +14105,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:69">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -13458,14 +14122,14 @@
         <v>65400</v>
       </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:69">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:69">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -13655,8 +14319,20 @@
       <c r="BM4" s="6">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:65">
+      <c r="BN4" s="6">
+        <v>63</v>
+      </c>
+      <c r="BO4" s="6">
+        <v>64</v>
+      </c>
+      <c r="BP4" s="6">
+        <v>65</v>
+      </c>
+      <c r="BQ4" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -13848,12 +14524,24 @@
       <c r="BM5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:65">
+      <c r="BN5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="BO5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="BP5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BQ5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-90662.510000000024</v>
+        <v>-86128.910000000018</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -14044,8 +14732,20 @@
       <c r="BM6" s="2">
         <v>997.84</v>
       </c>
-    </row>
-    <row r="7" spans="1:65">
+      <c r="BN6" s="2">
+        <v>-961.35</v>
+      </c>
+      <c r="BO6" s="2">
+        <v>1888.03</v>
+      </c>
+      <c r="BP6" s="2">
+        <v>1841.85</v>
+      </c>
+      <c r="BQ6" s="2">
+        <v>1765.07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -14237,8 +14937,20 @@
       <c r="BM7" s="2">
         <v>989.95</v>
       </c>
-    </row>
-    <row r="8" spans="1:65">
+      <c r="BN7" s="2">
+        <v>-3271.85</v>
+      </c>
+      <c r="BO7" s="2">
+        <v>-355.04</v>
+      </c>
+      <c r="BP7" s="2">
+        <v>1206.6600000000001</v>
+      </c>
+      <c r="BQ7" s="2">
+        <v>-1850.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -14430,8 +15142,20 @@
       <c r="BM8" s="2">
         <v>7.89</v>
       </c>
-    </row>
-    <row r="9" spans="1:65">
+      <c r="BN8" s="2">
+        <v>2310.4899999999998</v>
+      </c>
+      <c r="BO8" s="2">
+        <v>2243.06</v>
+      </c>
+      <c r="BP8" s="2">
+        <v>635.19000000000005</v>
+      </c>
+      <c r="BQ8" s="2">
+        <v>3616.07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -14623,15 +15347,27 @@
       <c r="BM9" s="13">
         <v>56.79</v>
       </c>
-    </row>
-    <row r="10" spans="1:65">
+      <c r="BN9" s="13">
+        <v>56.29</v>
+      </c>
+      <c r="BO9" s="13">
+        <v>57.65</v>
+      </c>
+      <c r="BP9" s="13">
+        <v>57.54</v>
+      </c>
+      <c r="BQ9" s="13">
+        <v>57.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-2.382330068097405E-2</v>
+        <v>-2.2628262011574002E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-1558.0438645357028</v>
+        <v>-1479.8883355569396</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -14881,11 +15617,27 @@
         <v>-76.888462942679809</v>
       </c>
       <c r="BM10" s="6">
-        <f t="shared" ref="BM10" si="28">BM6/BM9</f>
+        <f t="shared" ref="BM10:BN10" si="28">BM6/BM9</f>
         <v>17.570699066737102</v>
       </c>
-    </row>
-    <row r="11" spans="1:65">
+      <c r="BN10" s="6">
+        <f t="shared" si="28"/>
+        <v>-17.078521939953813</v>
+      </c>
+      <c r="BO10" s="6">
+        <f>BO6/BO9</f>
+        <v>32.749869904596707</v>
+      </c>
+      <c r="BP10" s="6">
+        <f>BP6/BP9</f>
+        <v>32.009906152241918</v>
+      </c>
+      <c r="BQ10" s="6">
+        <f>BQ6/BQ9</f>
+        <v>30.474274861878452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -15139,8 +15891,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-90662.510000000024</v>
       </c>
-    </row>
-    <row r="12" spans="1:65">
+      <c r="BN11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-91623.86000000003</v>
+      </c>
+      <c r="BO11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-89735.830000000031</v>
+      </c>
+      <c r="BP11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-87893.980000000025</v>
+      </c>
+      <c r="BQ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-86128.910000000018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -15394,8 +16162,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-72263.819999999978</v>
       </c>
-    </row>
-    <row r="13" spans="1:65">
+      <c r="BN12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-75535.669999999984</v>
+      </c>
+      <c r="BO12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-75890.709999999977</v>
+      </c>
+      <c r="BP12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-74684.049999999974</v>
+      </c>
+      <c r="BQ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-76535.039999999979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -15649,19 +16433,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-18398.729999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:65">
+      <c r="BN13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-16088.239999999996</v>
+      </c>
+      <c r="BO13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-13845.179999999997</v>
+      </c>
+      <c r="BP13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-13209.989999999996</v>
+      </c>
+      <c r="BQ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-9593.9199999999964</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>58.18995990014534</v>
+        <v>58.1996005580964</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:69">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -15669,7 +16469,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:69">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -15877,10 +16677,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM49"/>
+  <dimension ref="A1:BQ49"/>
   <sheetViews>
     <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BM7" sqref="BM7"/>
+      <selection activeCell="BQ7" sqref="BQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15889,7 +16689,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:69">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -15897,7 +16697,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:69">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -15914,14 +16714,14 @@
         <v>104100</v>
       </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:69">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:69">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -16111,8 +16911,20 @@
       <c r="BM4" s="6">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:65">
+      <c r="BN4" s="6">
+        <v>63</v>
+      </c>
+      <c r="BO4" s="6">
+        <v>64</v>
+      </c>
+      <c r="BP4" s="6">
+        <v>65</v>
+      </c>
+      <c r="BQ4" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -16304,12 +17116,24 @@
       <c r="BM5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:65">
+      <c r="BN5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="BO5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="BP5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BQ5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-3011.81</v>
+        <v>-11178.280000000002</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -16500,8 +17324,20 @@
       <c r="BM6" s="2">
         <v>1688.98</v>
       </c>
-    </row>
-    <row r="7" spans="1:65">
+      <c r="BN6" s="2">
+        <v>195.91</v>
+      </c>
+      <c r="BO6" s="2">
+        <v>-1631.04</v>
+      </c>
+      <c r="BP6" s="2">
+        <v>-4074.3</v>
+      </c>
+      <c r="BQ6" s="2">
+        <v>-2657.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -16693,8 +17529,20 @@
       <c r="BM7" s="2">
         <v>417.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:65">
+      <c r="BN7" s="2">
+        <v>-283.2</v>
+      </c>
+      <c r="BO7" s="2">
+        <v>-2000.02</v>
+      </c>
+      <c r="BP7" s="2">
+        <v>-3476.72</v>
+      </c>
+      <c r="BQ7" s="2">
+        <v>-814.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -16886,8 +17734,20 @@
       <c r="BM8" s="2">
         <v>1271.0899999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:65">
+      <c r="BN8" s="2">
+        <v>479.11</v>
+      </c>
+      <c r="BO8" s="2">
+        <v>368.98</v>
+      </c>
+      <c r="BP8" s="2">
+        <v>-597.61</v>
+      </c>
+      <c r="BQ8" s="2">
+        <v>-1842.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -17079,15 +17939,27 @@
       <c r="BM9" s="13">
         <v>116.11</v>
       </c>
-    </row>
-    <row r="10" spans="1:65">
+      <c r="BN9" s="13">
+        <v>116.96</v>
+      </c>
+      <c r="BO9" s="13">
+        <v>118.45</v>
+      </c>
+      <c r="BP9" s="13">
+        <v>110.03</v>
+      </c>
+      <c r="BQ9" s="13">
+        <v>108.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-4.2362756313462182E-4</v>
+        <v>-1.1312616240474402E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-44.099629322314129</v>
+        <v>-117.76433506333852</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -17340,8 +18212,24 @@
         <f>BM6/BM9</f>
         <v>14.54637843424339</v>
       </c>
-    </row>
-    <row r="11" spans="1:65">
+      <c r="BN10" s="6">
+        <f>BN6/BN9</f>
+        <v>1.6750170998632012</v>
+      </c>
+      <c r="BO10" s="6">
+        <f>BO6/BO9</f>
+        <v>-13.769860700717603</v>
+      </c>
+      <c r="BP10" s="6">
+        <f>BP6/BP9</f>
+        <v>-37.028992093065526</v>
+      </c>
+      <c r="BQ10" s="6">
+        <f>BQ6/BQ9</f>
+        <v>-24.540870047104463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -17595,8 +18483,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-3011.81</v>
       </c>
-    </row>
-    <row r="12" spans="1:65">
+      <c r="BN11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-2815.9</v>
+      </c>
+      <c r="BO11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-4446.9400000000005</v>
+      </c>
+      <c r="BP11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-8521.2400000000016</v>
+      </c>
+      <c r="BQ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-11178.280000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -17850,8 +18754,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>12624.069999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:65">
+      <c r="BN12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>12340.869999999995</v>
+      </c>
+      <c r="BO12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>10340.849999999995</v>
+      </c>
+      <c r="BP12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>6864.1299999999956</v>
+      </c>
+      <c r="BQ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>6050.0099999999957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -18105,19 +19025,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-15667.599999999984</v>
       </c>
-    </row>
-    <row r="14" spans="1:65">
+      <c r="BN13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-15188.489999999983</v>
+      </c>
+      <c r="BO13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-14819.509999999984</v>
+      </c>
+      <c r="BP13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-15417.119999999984</v>
+      </c>
+      <c r="BQ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-17260.049999999985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>68.295585388878621</v>
+        <v>94.920758428159616</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:69">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -18125,7 +19061,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:69">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -18333,10 +19269,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW49"/>
+  <dimension ref="A1:BA49"/>
   <sheetViews>
     <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+      <selection activeCell="BA7" sqref="BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18345,7 +19281,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:53">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -18353,7 +19289,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:53">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -18370,14 +19306,14 @@
         <v>9555800</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:53">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:53">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -18519,8 +19455,20 @@
       <c r="AW4" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:49">
+      <c r="AX4" s="6">
+        <v>47</v>
+      </c>
+      <c r="AY4" s="6">
+        <v>48</v>
+      </c>
+      <c r="AZ4" s="6">
+        <v>49</v>
+      </c>
+      <c r="BA4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -18664,12 +19612,24 @@
       <c r="AW5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:49">
+      <c r="AX5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>3469.0200000000159</v>
+        <v>-9860.6499999999833</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -18812,8 +19772,20 @@
       <c r="AW6" s="2">
         <v>-5028.88</v>
       </c>
-    </row>
-    <row r="7" spans="1:49">
+      <c r="AX6" s="2">
+        <v>-6846.04</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>-3395.6</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>1024.3900000000001</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>-4112.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -18957,8 +19929,20 @@
       <c r="AW7" s="2">
         <v>511.06</v>
       </c>
-    </row>
-    <row r="8" spans="1:49">
+      <c r="AX7" s="2">
+        <v>-10566.75</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>-1970.13</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>-2803.79</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>-4236.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -19102,8 +20086,20 @@
       <c r="AW8" s="2">
         <v>-5539.93</v>
       </c>
-    </row>
-    <row r="9" spans="1:49">
+      <c r="AX8" s="2">
+        <v>3720.72</v>
+      </c>
+      <c r="AY8" s="2">
+        <v>-1425.46</v>
+      </c>
+      <c r="AZ8" s="2">
+        <v>3828.19</v>
+      </c>
+      <c r="BA8" s="2">
+        <v>123.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -19247,15 +20243,27 @@
       <c r="AW9" s="13">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:49">
+      <c r="AX9" s="13">
+        <v>6.96</v>
+      </c>
+      <c r="AY9" s="13">
+        <v>6.92</v>
+      </c>
+      <c r="AZ9" s="13">
+        <v>6.95</v>
+      </c>
+      <c r="BA9" s="13">
+        <v>6.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>4.0940608017368452E-5</v>
+        <v>-1.6093020422105046E-4</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>391.22026209236947</v>
+        <v>-1537.8168454955139</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -19444,8 +20452,24 @@
         <f t="shared" si="20"/>
         <v>-718.41142857142859</v>
       </c>
-    </row>
-    <row r="11" spans="1:49">
+      <c r="AX10" s="6">
+        <f t="shared" ref="AX10:AY10" si="21">AX6/AX9</f>
+        <v>-983.62643678160919</v>
+      </c>
+      <c r="AY10" s="6">
+        <f t="shared" si="21"/>
+        <v>-490.69364161849711</v>
+      </c>
+      <c r="AZ10" s="6">
+        <f t="shared" ref="AZ10:BA10" si="22">AZ6/AZ9</f>
+        <v>147.39424460431655</v>
+      </c>
+      <c r="BA10" s="6">
+        <f t="shared" si="22"/>
+        <v>-602.1112737920937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -19635,8 +20659,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>3469.0200000000159</v>
       </c>
-    </row>
-    <row r="12" spans="1:49">
+      <c r="AX11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-3377.0199999999841</v>
+      </c>
+      <c r="AY11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-6772.6199999999844</v>
+      </c>
+      <c r="AZ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-5748.2299999999841</v>
+      </c>
+      <c r="BA11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-9860.6499999999833</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -19826,8 +20866,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>86152.15</v>
       </c>
-    </row>
-    <row r="13" spans="1:49">
+      <c r="AX12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>75585.399999999994</v>
+      </c>
+      <c r="AY12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>73615.26999999999</v>
+      </c>
+      <c r="AZ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>70811.48</v>
+      </c>
+      <c r="BA12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>66575.26999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -20017,19 +21073,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-82757.050000000017</v>
       </c>
-    </row>
-    <row r="14" spans="1:49">
+      <c r="AX13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-79036.330000000016</v>
+      </c>
+      <c r="AY13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-80461.790000000023</v>
+      </c>
+      <c r="AZ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-76633.60000000002</v>
+      </c>
+      <c r="BA13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-76509.810000000027</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>8.8671787638160708</v>
+        <v>6.4121094972286468</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:53">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -20037,7 +21109,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:53">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -20245,10 +21317,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW49"/>
+  <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="BA7" sqref="BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20257,7 +21329,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:53">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -20265,7 +21337,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:53">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -20282,14 +21354,14 @@
         <v>2209000</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:53">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:53">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -20431,8 +21503,20 @@
       <c r="AW4" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:49">
+      <c r="AX4" s="6">
+        <v>47</v>
+      </c>
+      <c r="AY4" s="6">
+        <v>48</v>
+      </c>
+      <c r="AZ4" s="6">
+        <v>49</v>
+      </c>
+      <c r="BA4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -20576,12 +21660,24 @@
       <c r="AW5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:49">
+      <c r="AX5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-84993.88</v>
+        <v>-89667.55</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -20724,8 +21820,20 @@
       <c r="AW6" s="2">
         <v>-721.92</v>
       </c>
-    </row>
-    <row r="7" spans="1:49">
+      <c r="AX6" s="2">
+        <v>-4176.3999999999996</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>-1233.8499999999999</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>6682.39</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>-5945.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -20869,8 +21977,20 @@
       <c r="AW7" s="2">
         <v>-2451.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:49">
+      <c r="AX7" s="2">
+        <v>-1948.31</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>-4033.47</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>8679.74</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>-7000.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -21014,8 +22134,20 @@
       <c r="AW8" s="2">
         <v>1729.93</v>
       </c>
-    </row>
-    <row r="9" spans="1:49">
+      <c r="AX8" s="2">
+        <v>-2228.09</v>
+      </c>
+      <c r="AY8" s="2">
+        <v>2799.62</v>
+      </c>
+      <c r="AZ8" s="2">
+        <v>-1997.36</v>
+      </c>
+      <c r="BA8" s="2">
+        <v>1054.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -21159,15 +22291,27 @@
       <c r="AW9" s="13">
         <v>8.4600000000000009</v>
       </c>
-    </row>
-    <row r="10" spans="1:49">
+      <c r="AX9" s="13">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="AY9" s="13">
+        <v>8.42</v>
+      </c>
+      <c r="AZ9" s="13">
+        <v>8.57</v>
+      </c>
+      <c r="BA9" s="13">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-4.4656248182283753E-3</v>
+        <v>-4.7287141917403842E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-9864.5652234664813</v>
+        <v>-10445.729649554509</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -21356,8 +22500,24 @@
         <f t="shared" si="22"/>
         <v>-85.333333333333314</v>
       </c>
-    </row>
-    <row r="11" spans="1:49">
+      <c r="AX10" s="6">
+        <f t="shared" ref="AX10:AY10" si="23">AX6/AX9</f>
+        <v>-493.66430260047269</v>
+      </c>
+      <c r="AY10" s="6">
+        <f t="shared" si="23"/>
+        <v>-146.53800475059381</v>
+      </c>
+      <c r="AZ10" s="6">
+        <f t="shared" ref="AZ10:BA10" si="24">AZ6/AZ9</f>
+        <v>779.74212368728126</v>
+      </c>
+      <c r="BA10" s="6">
+        <f t="shared" si="24"/>
+        <v>-720.70424242424247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -21547,8 +22707,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-84993.88</v>
       </c>
-    </row>
-    <row r="12" spans="1:49">
+      <c r="AX11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-89170.28</v>
+      </c>
+      <c r="AY11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-90404.13</v>
+      </c>
+      <c r="AZ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-83721.740000000005</v>
+      </c>
+      <c r="BA11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-89667.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -21738,8 +22914,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-44359.459999999985</v>
       </c>
-    </row>
-    <row r="13" spans="1:49">
+      <c r="AX12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-46307.769999999982</v>
+      </c>
+      <c r="AY12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-50341.239999999983</v>
+      </c>
+      <c r="AZ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-41661.499999999985</v>
+      </c>
+      <c r="BA12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-48662.079999999987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -21929,19 +23121,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-41741.869999999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:49">
+      <c r="AX13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-43969.959999999992</v>
+      </c>
+      <c r="AY13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-41170.339999999989</v>
+      </c>
+      <c r="AZ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-43167.69999999999</v>
+      </c>
+      <c r="BA13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-42112.919999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>8.6160796826413524</v>
+        <v>8.5841346663441698</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:53">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -21949,7 +23157,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:53">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -22157,10 +23365,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW49"/>
+  <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="BA7" sqref="BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22169,7 +23377,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:53">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -22177,7 +23385,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:53">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -22194,14 +23402,14 @@
         <v>4010.0000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:53">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:53">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -22343,8 +23551,20 @@
       <c r="AW4" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:49">
+      <c r="AX4" s="6">
+        <v>47</v>
+      </c>
+      <c r="AY4" s="6">
+        <v>48</v>
+      </c>
+      <c r="AZ4" s="6">
+        <v>49</v>
+      </c>
+      <c r="BA4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -22488,12 +23708,24 @@
       <c r="AW5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:49">
+      <c r="AX5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-50425.09</v>
+        <v>-58578.47</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -22636,8 +23868,20 @@
       <c r="AW6" s="2">
         <v>184.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:49">
+      <c r="AX6" s="2">
+        <v>-2899.41</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>-882.97</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>-1135.54</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>-3235.46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -22781,8 +24025,20 @@
       <c r="AW7" s="2">
         <v>292.73</v>
       </c>
-    </row>
-    <row r="8" spans="1:49">
+      <c r="AX7" s="2">
+        <v>-1474.37</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>-847.13</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>-192.76</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>-1779.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -22926,8 +24182,20 @@
       <c r="AW8" s="2">
         <v>-107.93</v>
       </c>
-    </row>
-    <row r="9" spans="1:49">
+      <c r="AX8" s="2">
+        <v>-1425.03</v>
+      </c>
+      <c r="AY8" s="2">
+        <v>-35.840000000000003</v>
+      </c>
+      <c r="AZ8" s="2">
+        <v>-942.78</v>
+      </c>
+      <c r="BA8" s="2">
+        <v>-1455.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -23071,15 +24339,27 @@
       <c r="AW9" s="13">
         <v>152.26</v>
       </c>
-    </row>
-    <row r="10" spans="1:49">
+      <c r="AX9" s="13">
+        <v>148.72</v>
+      </c>
+      <c r="AY9" s="13">
+        <v>147.9</v>
+      </c>
+      <c r="AZ9" s="13">
+        <v>145.97</v>
+      </c>
+      <c r="BA9" s="13">
+        <v>137.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-8.1203536263121379E-2</v>
+        <v>-9.537789752863314E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-325.62618041511678</v>
+        <v>-382.46536908981892</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -23268,8 +24548,24 @@
         <f t="shared" si="22"/>
         <v>1.2137133849993433</v>
       </c>
-    </row>
-    <row r="11" spans="1:49">
+      <c r="AX10" s="6">
+        <f t="shared" ref="AX10:AY10" si="23">AX6/AX9</f>
+        <v>-19.495763851533081</v>
+      </c>
+      <c r="AY10" s="6">
+        <f t="shared" si="23"/>
+        <v>-5.9700473292765386</v>
+      </c>
+      <c r="AZ10" s="6">
+        <f t="shared" ref="AZ10:BA10" si="24">AZ6/AZ9</f>
+        <v>-7.7792697129547168</v>
+      </c>
+      <c r="BA10" s="6">
+        <f t="shared" si="24"/>
+        <v>-23.594107780937797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -23459,8 +24755,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-50425.09</v>
       </c>
-    </row>
-    <row r="12" spans="1:49">
+      <c r="AX11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-53324.5</v>
+      </c>
+      <c r="AY11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-54207.47</v>
+      </c>
+      <c r="AZ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-55343.01</v>
+      </c>
+      <c r="BA11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-58578.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -23650,8 +24962,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-28594.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:49">
+      <c r="AX12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-30068.379999999997</v>
+      </c>
+      <c r="AY12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-30915.51</v>
+      </c>
+      <c r="AZ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-31108.269999999997</v>
+      </c>
+      <c r="BA12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-32888.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -23841,19 +25169,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-20565.060000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:49">
+      <c r="AX13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-21990.09</v>
+      </c>
+      <c r="AY13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-22025.93</v>
+      </c>
+      <c r="AZ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-22968.71</v>
+      </c>
+      <c r="BA13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-24424.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>154.85576109303241</v>
+        <v>153.16019366512452</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:53">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -23861,7 +25205,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:53">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -24069,10 +25413,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW49"/>
+  <dimension ref="A1:BA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="BA7" sqref="BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24081,7 +25425,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:53">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -24089,7 +25433,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:53">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -24106,14 +25450,14 @@
         <v>113800.00000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:53">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:53">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -24255,8 +25599,20 @@
       <c r="AW4" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:49">
+      <c r="AX4" s="6">
+        <v>47</v>
+      </c>
+      <c r="AY4" s="6">
+        <v>48</v>
+      </c>
+      <c r="AZ4" s="6">
+        <v>49</v>
+      </c>
+      <c r="BA4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -24400,12 +25756,24 @@
       <c r="AW5" s="5">
         <v>43244</v>
       </c>
-    </row>
-    <row r="6" spans="1:49">
+      <c r="AX5" s="5">
+        <v>43245</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>43248</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>43249</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-122336.52</v>
+        <v>-135147.51999999999</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -24548,8 +25916,20 @@
       <c r="AW6" s="2">
         <v>-713.63</v>
       </c>
-    </row>
-    <row r="7" spans="1:49">
+      <c r="AX6" s="2">
+        <v>-428.95</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>-3956.06</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>-1930.61</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>-6495.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -24693,8 +26073,20 @@
       <c r="AW7" s="2">
         <v>-1377.01</v>
       </c>
-    </row>
-    <row r="8" spans="1:49">
+      <c r="AX7" s="2">
+        <v>-1520.35</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>-2983.13</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>-2338.4299999999998</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>-3385.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -24838,8 +26230,20 @@
       <c r="AW8" s="2">
         <v>663.39</v>
       </c>
-    </row>
-    <row r="9" spans="1:49">
+      <c r="AX8" s="2">
+        <v>1091.4000000000001</v>
+      </c>
+      <c r="AY8" s="2">
+        <v>-972.93</v>
+      </c>
+      <c r="AZ8" s="2">
+        <v>407.81</v>
+      </c>
+      <c r="BA8" s="2">
+        <v>-3110.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -24983,15 +26387,27 @@
       <c r="AW9" s="13">
         <v>54.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:49">
+      <c r="AX9" s="13">
+        <v>54.22</v>
+      </c>
+      <c r="AY9" s="13">
+        <v>52.78</v>
+      </c>
+      <c r="AZ9" s="13">
+        <v>53.5</v>
+      </c>
+      <c r="BA9" s="13">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-1.92826950241742E-2</v>
+        <v>-2.146044382242808E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-2194.3706937510242</v>
+        <v>-2442.1985069923157</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -25157,31 +26573,47 @@
         <v>1.5913059984813971</v>
       </c>
       <c r="AR10" s="6">
-        <f>AR6/AR9</f>
+        <f t="shared" ref="AR10:BA10" si="20">AR6/AR9</f>
         <v>1.694712905059693</v>
       </c>
       <c r="AS10" s="6">
-        <f>AS6/AS9</f>
+        <f t="shared" si="20"/>
         <v>-63.1575925925926</v>
       </c>
       <c r="AT10" s="6">
-        <f>AT6/AT9</f>
+        <f t="shared" si="20"/>
         <v>0.16061606160616063</v>
       </c>
       <c r="AU10" s="6">
-        <f>AU6/AU9</f>
+        <f t="shared" si="20"/>
         <v>21.211090909090906</v>
       </c>
       <c r="AV10" s="6">
-        <f>AV6/AV9</f>
+        <f t="shared" si="20"/>
         <v>13.775054864667155</v>
       </c>
       <c r="AW10" s="6">
-        <f>AW6/AW9</f>
+        <f t="shared" si="20"/>
         <v>-13.178762696214219</v>
       </c>
-    </row>
-    <row r="11" spans="1:49">
+      <c r="AX10" s="6">
+        <f t="shared" si="20"/>
+        <v>-7.9112873478421246</v>
+      </c>
+      <c r="AY10" s="6">
+        <f t="shared" si="20"/>
+        <v>-74.953770367563465</v>
+      </c>
+      <c r="AZ10" s="6">
+        <f t="shared" si="20"/>
+        <v>-36.086168224299065</v>
+      </c>
+      <c r="BA10" s="6">
+        <f t="shared" si="20"/>
+        <v>-128.87658730158731</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -25371,8 +26803,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-122336.52</v>
       </c>
-    </row>
-    <row r="12" spans="1:49">
+      <c r="AX11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-122765.47</v>
+      </c>
+      <c r="AY11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-126721.53</v>
+      </c>
+      <c r="AZ11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-128652.14</v>
+      </c>
+      <c r="BA11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-135147.51999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -25562,8 +27010,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-143822.74000000005</v>
       </c>
-    </row>
-    <row r="13" spans="1:49">
+      <c r="AX12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-145343.09000000005</v>
+      </c>
+      <c r="AY12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-148326.22000000006</v>
+      </c>
+      <c r="AZ12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-150664.65000000005</v>
+      </c>
+      <c r="BA12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-154049.73000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -25753,19 +27217,35 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>28306.989999999987</v>
       </c>
-    </row>
-    <row r="14" spans="1:49">
+      <c r="AX13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>29398.389999999989</v>
+      </c>
+      <c r="AY13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>28425.459999999988</v>
+      </c>
+      <c r="AZ13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>28833.26999999999</v>
+      </c>
+      <c r="BA13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>25722.979999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>55.750161241389804</v>
+        <v>55.338466391268341</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:53">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -25773,7 +27253,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:53">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
2018-5-31 ~ 2018-6-1 update
</commit_message>
<xml_diff>
--- a/stock_vip.xlsx
+++ b/stock_vip.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="1000" activeTab="7"/>
+    <workbookView xWindow="2700" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="1000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="美的集团" sheetId="21" r:id="rId1"/>
@@ -890,6 +890,12 @@
                 <c:pt idx="65">
                   <c:v>50.71</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>52.91</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>52.15</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -905,11 +911,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081511208"/>
-        <c:axId val="2081981032"/>
+        <c:axId val="2088262888"/>
+        <c:axId val="2089970936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081511208"/>
+        <c:axId val="2088262888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -918,7 +924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081981032"/>
+        <c:crossAx val="2089970936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -926,7 +932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081981032"/>
+        <c:axId val="2089970936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45.0"/>
@@ -938,7 +944,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081511208"/>
+        <c:crossAx val="2088262888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1137,6 +1143,12 @@
                 <c:pt idx="49">
                   <c:v>-9860.649999999983</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-5896.109999999983</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-8561.649999999983</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1304,6 +1316,12 @@
                 <c:pt idx="49">
                   <c:v>66575.26999999999</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>61968.06</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>60783.19999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1471,6 +1489,12 @@
                 <c:pt idx="49">
                   <c:v>-76509.81000000003</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-67938.07000000002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-69418.76000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1486,11 +1510,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081998168"/>
-        <c:axId val="2104678232"/>
+        <c:axId val="-2064185400"/>
+        <c:axId val="-2064182424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081998168"/>
+        <c:axId val="-2064185400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104678232"/>
+        <c:crossAx val="-2064182424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104678232"/>
+        <c:axId val="-2064182424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081998168"/>
+        <c:crossAx val="-2064185400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1717,6 +1741,12 @@
                 <c:pt idx="49">
                   <c:v>8.25</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.42</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.35</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1732,11 +1762,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082171944"/>
-        <c:axId val="2046902648"/>
+        <c:axId val="2053310776"/>
+        <c:axId val="2053113224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082171944"/>
+        <c:axId val="2053310776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046902648"/>
+        <c:crossAx val="2053113224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1753,7 +1783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2046902648"/>
+        <c:axId val="2053113224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,7 +1794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082171944"/>
+        <c:crossAx val="2053310776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1963,6 +1993,12 @@
                 <c:pt idx="49">
                   <c:v>-89667.55</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-87729.90000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-84750.59000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2130,6 +2166,12 @@
                 <c:pt idx="49">
                   <c:v>-48662.07999999998</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-47948.14999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-51850.04999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2297,6 +2339,12 @@
                 <c:pt idx="49">
                   <c:v>-42112.92</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-40889.18999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-34007.96999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2312,11 +2360,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082232376"/>
-        <c:axId val="2105408760"/>
+        <c:axId val="2053892360"/>
+        <c:axId val="2086176424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082232376"/>
+        <c:axId val="2053892360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2325,7 +2373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105408760"/>
+        <c:crossAx val="2086176424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2333,7 +2381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105408760"/>
+        <c:axId val="2086176424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082232376"/>
+        <c:crossAx val="2053892360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2543,6 +2591,12 @@
                 <c:pt idx="49">
                   <c:v>137.13</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>139.02</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>135.14</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2558,11 +2612,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082234104"/>
-        <c:axId val="2104883096"/>
+        <c:axId val="2094088584"/>
+        <c:axId val="-2135342936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082234104"/>
+        <c:axId val="2094088584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,7 +2625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104883096"/>
+        <c:crossAx val="-2135342936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2579,7 +2633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104883096"/>
+        <c:axId val="-2135342936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="130.0"/>
@@ -2591,7 +2645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082234104"/>
+        <c:crossAx val="2094088584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2790,6 +2844,12 @@
                 <c:pt idx="49">
                   <c:v>-58578.47</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-58546.63</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-60422.91</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2957,6 +3017,12 @@
                 <c:pt idx="49">
                   <c:v>-32888.14</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-32556.3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-33912.9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3124,6 +3190,12 @@
                 <c:pt idx="49">
                   <c:v>-24424.3</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-24724.3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-25243.99</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3139,11 +3211,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105125800"/>
-        <c:axId val="2046980392"/>
+        <c:axId val="-2135300408"/>
+        <c:axId val="-2135297432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105125800"/>
+        <c:axId val="-2135300408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3152,7 +3224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046980392"/>
+        <c:crossAx val="-2135297432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3160,7 +3232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2046980392"/>
+        <c:axId val="-2135297432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3171,7 +3243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105125800"/>
+        <c:crossAx val="-2135300408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3370,6 +3442,12 @@
                 <c:pt idx="49">
                   <c:v>50.4</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.15</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50.91</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3385,11 +3463,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082446472"/>
-        <c:axId val="2048106104"/>
+        <c:axId val="-2135251672"/>
+        <c:axId val="-2135248664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082446472"/>
+        <c:axId val="-2135251672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3398,7 +3476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048106104"/>
+        <c:crossAx val="-2135248664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3406,7 +3484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2048106104"/>
+        <c:axId val="-2135248664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45.0"/>
@@ -3418,7 +3496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082446472"/>
+        <c:crossAx val="-2135251672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3617,6 +3695,12 @@
                 <c:pt idx="49">
                   <c:v>-135147.52</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-137283.17</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-139029.33</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3784,6 +3868,12 @@
                 <c:pt idx="49">
                   <c:v>-154049.73</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>-155049.73</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-155499.4300000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3951,6 +4041,12 @@
                 <c:pt idx="49">
                   <c:v>25722.97999999999</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>24587.32999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23290.86999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3966,11 +4062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2104600296"/>
-        <c:axId val="2105268312"/>
+        <c:axId val="-2135206472"/>
+        <c:axId val="-2135203496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2104600296"/>
+        <c:axId val="-2135206472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3979,7 +4075,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105268312"/>
+        <c:crossAx val="-2135203496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3987,7 +4083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105268312"/>
+        <c:axId val="-2135203496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3998,7 +4094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104600296"/>
+        <c:crossAx val="-2135206472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4245,6 +4341,12 @@
                 <c:pt idx="65">
                   <c:v>-197640.66</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-187121.83</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-194982.32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4460,6 +4562,12 @@
                 <c:pt idx="65">
                   <c:v>-51520.22000000002</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-35524.29000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-47987.62000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4675,6 +4783,12 @@
                 <c:pt idx="65">
                   <c:v>-146119.58</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-151596.69</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-146993.82</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4690,11 +4804,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2047266728"/>
-        <c:axId val="2105444024"/>
+        <c:axId val="-2135632952"/>
+        <c:axId val="-2135629976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2047266728"/>
+        <c:axId val="-2135632952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4703,7 +4817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105444024"/>
+        <c:crossAx val="-2135629976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4711,7 +4825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105444024"/>
+        <c:axId val="-2135629976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4722,7 +4836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047266728"/>
+        <c:crossAx val="-2135632952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4969,6 +5083,12 @@
                 <c:pt idx="65">
                   <c:v>725.87</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>751.13</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>745.11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4984,11 +5104,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105034136"/>
-        <c:axId val="2081492392"/>
+        <c:axId val="2090002792"/>
+        <c:axId val="2089981784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105034136"/>
+        <c:axId val="2090002792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4997,7 +5117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081492392"/>
+        <c:crossAx val="2089981784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5005,7 +5125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081492392"/>
+        <c:axId val="2089981784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5016,7 +5136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105034136"/>
+        <c:crossAx val="2090002792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5263,6 +5383,12 @@
                 <c:pt idx="65">
                   <c:v>12485.82</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>13180.17</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>13664.01</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5478,6 +5604,12 @@
                 <c:pt idx="65">
                   <c:v>-77061.21</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-44731.96999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-70729.87</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5693,6 +5825,12 @@
                 <c:pt idx="65">
                   <c:v>89547.30000000001</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>57912.29000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>84393.99000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5708,11 +5846,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081667912"/>
-        <c:axId val="2047964664"/>
+        <c:axId val="-2063911576"/>
+        <c:axId val="-2063908600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081667912"/>
+        <c:axId val="-2063911576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5721,7 +5859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047964664"/>
+        <c:crossAx val="-2063908600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5729,7 +5867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047964664"/>
+        <c:axId val="-2063908600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5740,7 +5878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081667912"/>
+        <c:crossAx val="-2063911576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5987,6 +6125,12 @@
                 <c:pt idx="65">
                   <c:v>57.92</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>60.02</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>59.39</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6002,11 +6146,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2104985016"/>
-        <c:axId val="2081798936"/>
+        <c:axId val="2082242984"/>
+        <c:axId val="2047891176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2104985016"/>
+        <c:axId val="2082242984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6015,7 +6159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081798936"/>
+        <c:crossAx val="2047891176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6023,7 +6167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081798936"/>
+        <c:axId val="2047891176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="47.0"/>
@@ -6035,7 +6179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104985016"/>
+        <c:crossAx val="2082242984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6282,6 +6426,12 @@
                 <c:pt idx="65">
                   <c:v>-86128.91000000002</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-82849.12000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-85665.20000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6497,6 +6647,12 @@
                 <c:pt idx="65">
                   <c:v>-76535.03999999997</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-77744.35999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-81432.60999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6712,6 +6868,12 @@
                 <c:pt idx="65">
                   <c:v>-9593.919999999996</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-5104.789999999996</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-4232.619999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6727,11 +6889,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081992760"/>
-        <c:axId val="2081989752"/>
+        <c:axId val="2082390264"/>
+        <c:axId val="2081769416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081992760"/>
+        <c:axId val="2082390264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6740,7 +6902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081989752"/>
+        <c:crossAx val="2081769416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6748,7 +6910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081989752"/>
+        <c:axId val="2081769416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6759,7 +6921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081992760"/>
+        <c:crossAx val="2082390264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7006,6 +7168,12 @@
                 <c:pt idx="65">
                   <c:v>108.27</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>114.1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>110.11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7021,11 +7189,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2046936264"/>
-        <c:axId val="2105511832"/>
+        <c:axId val="-2063903368"/>
+        <c:axId val="-2063897336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2046936264"/>
+        <c:axId val="-2063903368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7034,7 +7202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105511832"/>
+        <c:crossAx val="-2063897336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7042,9 +7210,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105511832"/>
+        <c:axId val="-2063897336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="90.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7053,7 +7222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046936264"/>
+        <c:crossAx val="-2063903368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7300,6 +7469,12 @@
                 <c:pt idx="65">
                   <c:v>-11178.28</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-11520.98</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-13870.55</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7515,6 +7690,12 @@
                 <c:pt idx="65">
                   <c:v>6050.009999999996</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>6553.449999999995</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6584.549999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7730,6 +7911,12 @@
                 <c:pt idx="65">
                   <c:v>-17260.04999999998</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>-18106.19999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-20486.86999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7745,11 +7932,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2047180888"/>
-        <c:axId val="2081700632"/>
+        <c:axId val="2082184984"/>
+        <c:axId val="2048068184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2047180888"/>
+        <c:axId val="2082184984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7758,7 +7945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081700632"/>
+        <c:crossAx val="2048068184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7766,7 +7953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081700632"/>
+        <c:axId val="2048068184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7777,7 +7964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047180888"/>
+        <c:crossAx val="2082184984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7976,6 +8163,12 @@
                 <c:pt idx="49">
                   <c:v>6.83</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.05</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7991,11 +8184,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2104760008"/>
-        <c:axId val="2105522472"/>
+        <c:axId val="-2064230344"/>
+        <c:axId val="-2064227336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2104760008"/>
+        <c:axId val="-2064230344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8004,7 +8197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105522472"/>
+        <c:crossAx val="-2064227336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8012,7 +8205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105522472"/>
+        <c:axId val="-2064227336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8023,7 +8216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104760008"/>
+        <c:crossAx val="-2064230344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8898,10 +9091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ49"/>
+  <dimension ref="A1:BS49"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BQ7" sqref="BQ7"/>
+    <sheetView topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="BS7" sqref="BS7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8910,7 +9103,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:71">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -8918,7 +9111,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:71">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8" t="s">
@@ -8935,7 +9128,7 @@
         <v>630800</v>
       </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:71">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="8" t="s">
@@ -8945,7 +9138,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:71">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -9147,8 +9340,14 @@
       <c r="BQ4" s="6">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:69">
+      <c r="BR4" s="6">
+        <v>67</v>
+      </c>
+      <c r="BS4" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -9352,12 +9551,18 @@
       <c r="BQ5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:69">
+      <c r="BR5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BS5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-197640.66</v>
+        <v>-194982.32</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -9560,8 +9765,14 @@
       <c r="BQ6" s="2">
         <v>-4703.72</v>
       </c>
-    </row>
-    <row r="7" spans="1:69">
+      <c r="BR6" s="2">
+        <v>10518.83</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>-7860.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -9765,8 +9976,14 @@
       <c r="BQ7" s="2">
         <v>-3036.63</v>
       </c>
-    </row>
-    <row r="8" spans="1:69">
+      <c r="BR7" s="2">
+        <v>15995.93</v>
+      </c>
+      <c r="BS7" s="2">
+        <v>-12463.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -9970,8 +10187,14 @@
       <c r="BQ8" s="2">
         <v>-1667.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:69">
+      <c r="BR8" s="2">
+        <v>-5477.11</v>
+      </c>
+      <c r="BS8" s="2">
+        <v>4602.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -10175,15 +10398,21 @@
       <c r="BQ9" s="13">
         <v>50.71</v>
       </c>
-    </row>
-    <row r="10" spans="1:69">
+      <c r="BR9" s="13">
+        <v>52.91</v>
+      </c>
+      <c r="BS9" s="13">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-6.0772408033788385E-3</v>
+        <v>-6.0010239196521551E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-3833.5234987713711</v>
+        <v>-3785.4458885165795</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -10417,43 +10646,51 @@
         <v>-332.55911144578317</v>
       </c>
       <c r="BI10" s="6">
-        <f>BI6/BI9</f>
+        <f t="shared" ref="BI10:BS10" si="26">BI6/BI9</f>
         <v>-72.403043236221933</v>
       </c>
       <c r="BJ10" s="6">
-        <f>BJ6/BJ9</f>
+        <f t="shared" si="26"/>
         <v>-104.40259499536609</v>
       </c>
       <c r="BK10" s="6">
-        <f>BK6/BK9</f>
+        <f t="shared" si="26"/>
         <v>-550.63366901007021</v>
       </c>
       <c r="BL10" s="6">
-        <f>BL6/BL9</f>
+        <f t="shared" si="26"/>
         <v>-234.83513513513512</v>
       </c>
       <c r="BM10" s="6">
-        <f>BM6/BM9</f>
+        <f t="shared" si="26"/>
         <v>-254.14891944990177</v>
       </c>
       <c r="BN10" s="6">
-        <f>BN6/BN9</f>
+        <f t="shared" si="26"/>
         <v>-192.49159913026287</v>
       </c>
       <c r="BO10" s="6">
-        <f>BO6/BO9</f>
+        <f t="shared" si="26"/>
         <v>53.391413169041208</v>
       </c>
       <c r="BP10" s="6">
-        <f>BP6/BP9</f>
+        <f t="shared" si="26"/>
         <v>-27.657214993202562</v>
       </c>
       <c r="BQ10" s="6">
-        <f>BQ6/BQ9</f>
+        <f t="shared" si="26"/>
         <v>-92.757247091303498</v>
       </c>
-    </row>
-    <row r="11" spans="1:69">
+      <c r="BR10" s="6">
+        <f t="shared" si="26"/>
+        <v>198.8060858060858</v>
+      </c>
+      <c r="BS10" s="6">
+        <f t="shared" si="26"/>
+        <v>-150.72847555129434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -10723,8 +10960,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-197640.66</v>
       </c>
-    </row>
-    <row r="12" spans="1:69">
+      <c r="BR11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-187121.83000000002</v>
+      </c>
+      <c r="BS11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-194982.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -10994,8 +11239,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-51520.220000000016</v>
       </c>
-    </row>
-    <row r="13" spans="1:69">
+      <c r="BR12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-35524.290000000015</v>
+      </c>
+      <c r="BS12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-47987.620000000017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -11265,19 +11518,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-146119.57999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:69">
+      <c r="BR13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-151596.68999999997</v>
+      </c>
+      <c r="BS13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-146993.81999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>51.555875440268736</v>
+        <v>51.508415584936188</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:71">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -11285,7 +11546,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:71">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -11493,10 +11754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ49"/>
+  <dimension ref="A1:BS49"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BQ7" sqref="BQ7"/>
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BS7" sqref="BS7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11505,7 +11766,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:71">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -11513,7 +11774,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:71">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -11530,14 +11791,14 @@
         <v>125600</v>
       </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:71">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:71">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -11739,8 +12000,14 @@
       <c r="BQ4" s="6">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:69">
+      <c r="BR4" s="6">
+        <v>67</v>
+      </c>
+      <c r="BS4" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -11944,12 +12211,18 @@
       <c r="BQ5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:69">
+      <c r="BR5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BS5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>12485.820000000002</v>
+        <v>13664.010000000002</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -12152,8 +12425,14 @@
       <c r="BQ6" s="2">
         <v>931.86</v>
       </c>
-    </row>
-    <row r="7" spans="1:69">
+      <c r="BR6" s="2">
+        <v>694.35</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>483.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -12357,8 +12636,14 @@
       <c r="BQ7" s="2">
         <v>-7678.12</v>
       </c>
-    </row>
-    <row r="8" spans="1:69">
+      <c r="BR7" s="2">
+        <v>32329.24</v>
+      </c>
+      <c r="BS7" s="2">
+        <v>-25997.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -12562,8 +12847,14 @@
       <c r="BQ8" s="2">
         <v>8609.8700000000008</v>
       </c>
-    </row>
-    <row r="9" spans="1:69">
+      <c r="BR8" s="2">
+        <v>-31635.01</v>
+      </c>
+      <c r="BS8" s="2">
+        <v>26481.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -12767,15 +13058,21 @@
       <c r="BQ9" s="13">
         <v>725.87</v>
       </c>
-    </row>
-    <row r="10" spans="1:69" s="9" customFormat="1">
+      <c r="BR9" s="13">
+        <v>751.13</v>
+      </c>
+      <c r="BS9" s="13">
+        <v>745.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71" s="9" customFormat="1">
       <c r="A10" s="19">
         <f>B10/F2</f>
-        <v>1.418333102846503E-4</v>
+        <v>1.543632546567419E-4</v>
       </c>
       <c r="B10" s="20">
         <f>SUM(D10:IX10)</f>
-        <v>17.814263771752078</v>
+        <v>19.388024784886781</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>3</v>
@@ -13041,11 +13338,19 @@
         <v>0.45696785748465341</v>
       </c>
       <c r="BQ10" s="18">
-        <f t="shared" ref="BQ10" si="30">BQ6/BQ9</f>
+        <f t="shared" ref="BQ10:BR10" si="30">BQ6/BQ9</f>
         <v>1.2837835976138978</v>
       </c>
-    </row>
-    <row r="11" spans="1:69">
+      <c r="BR10" s="18">
+        <f t="shared" si="30"/>
+        <v>0.92440722644548878</v>
+      </c>
+      <c r="BS10" s="18">
+        <f t="shared" ref="BS10" si="31">BS6/BS9</f>
+        <v>0.64935378668921362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -13315,8 +13620,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>12485.820000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:69">
+      <c r="BR11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>13180.170000000002</v>
+      </c>
+      <c r="BS11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>13664.010000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -13586,8 +13899,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-77061.209999999992</v>
       </c>
-    </row>
-    <row r="13" spans="1:69">
+      <c r="BR12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-44731.969999999987</v>
+      </c>
+      <c r="BS12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-70729.87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -13857,19 +14178,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>89547.300000000017</v>
       </c>
-    </row>
-    <row r="14" spans="1:69">
+      <c r="BR13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>57912.290000000023</v>
+      </c>
+      <c r="BS13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>84393.99000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>700.88891463472419</v>
+        <v>704.76544937425888</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:71">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -13877,7 +14206,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:71">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -14085,10 +14414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ49"/>
+  <dimension ref="A1:BS49"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BQ6" sqref="BQ6"/>
+    <sheetView topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BS7" sqref="BS7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14097,7 +14426,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:71">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -14105,7 +14434,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:71">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -14122,14 +14451,14 @@
         <v>65400</v>
       </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:71">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:71">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -14331,8 +14660,14 @@
       <c r="BQ4" s="6">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:69">
+      <c r="BR4" s="6">
+        <v>67</v>
+      </c>
+      <c r="BS4" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -14536,12 +14871,18 @@
       <c r="BQ5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:69">
+      <c r="BR5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BS5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-86128.910000000018</v>
+        <v>-85665.200000000026</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -14744,8 +15085,14 @@
       <c r="BQ6" s="2">
         <v>1765.07</v>
       </c>
-    </row>
-    <row r="7" spans="1:69">
+      <c r="BR6" s="2">
+        <v>3279.79</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>-2816.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -14949,8 +15296,14 @@
       <c r="BQ7" s="2">
         <v>-1850.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:69">
+      <c r="BR7" s="2">
+        <v>-1209.32</v>
+      </c>
+      <c r="BS7" s="2">
+        <v>-3688.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -15154,8 +15507,14 @@
       <c r="BQ8" s="2">
         <v>3616.07</v>
       </c>
-    </row>
-    <row r="9" spans="1:69">
+      <c r="BR8" s="2">
+        <v>4489.13</v>
+      </c>
+      <c r="BS8" s="2">
+        <v>872.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -15359,15 +15718,21 @@
       <c r="BQ9" s="13">
         <v>57.92</v>
       </c>
-    </row>
-    <row r="10" spans="1:69">
+      <c r="BR9" s="13">
+        <v>60.02</v>
+      </c>
+      <c r="BS9" s="13">
+        <v>59.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-2.2628262011574002E-2</v>
+        <v>-2.2517738848601657E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-1479.8883355569396</v>
+        <v>-1472.6601206985483</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -15636,8 +16001,16 @@
         <f>BQ6/BQ9</f>
         <v>30.474274861878452</v>
       </c>
-    </row>
-    <row r="11" spans="1:69">
+      <c r="BR10" s="6">
+        <f>BR6/BR9</f>
+        <v>54.644951682772408</v>
+      </c>
+      <c r="BS10" s="6">
+        <f>BS6/BS9</f>
+        <v>-47.416736824381211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -15907,8 +16280,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-86128.910000000018</v>
       </c>
-    </row>
-    <row r="12" spans="1:69">
+      <c r="BR11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-82849.120000000024</v>
+      </c>
+      <c r="BS11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-85665.200000000026</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -16178,8 +16559,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-76535.039999999979</v>
       </c>
-    </row>
-    <row r="13" spans="1:69">
+      <c r="BR12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-77744.359999999986</v>
+      </c>
+      <c r="BS12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-81432.609999999986</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -16449,19 +16838,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-9593.9199999999964</v>
       </c>
-    </row>
-    <row r="14" spans="1:69">
+      <c r="BR13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-5104.7899999999963</v>
+      </c>
+      <c r="BS13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-4232.6199999999963</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>58.1996005580964</v>
+        <v>58.170380793203798</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:71">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -16469,7 +16866,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:71">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -16677,10 +17074,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ49"/>
+  <dimension ref="A1:BS49"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BQ7" sqref="BQ7"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BM39" sqref="BM39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16689,7 +17086,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:71">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -16697,7 +17094,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:71">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -16714,14 +17111,14 @@
         <v>104100</v>
       </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:71">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:71">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -16923,8 +17320,14 @@
       <c r="BQ4" s="6">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:69">
+      <c r="BR4" s="6">
+        <v>67</v>
+      </c>
+      <c r="BS4" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -17128,12 +17531,18 @@
       <c r="BQ5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:69">
+      <c r="BR5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BS5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-11178.280000000002</v>
+        <v>-13870.550000000003</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -17336,8 +17745,14 @@
       <c r="BQ6" s="2">
         <v>-2657.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:69">
+      <c r="BR6" s="2">
+        <v>-342.7</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>-2349.5700000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -17541,8 +17956,14 @@
       <c r="BQ7" s="2">
         <v>-814.12</v>
       </c>
-    </row>
-    <row r="8" spans="1:69">
+      <c r="BR7" s="2">
+        <v>503.44</v>
+      </c>
+      <c r="BS7" s="2">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -17746,8 +18167,14 @@
       <c r="BQ8" s="2">
         <v>-1842.93</v>
       </c>
-    </row>
-    <row r="9" spans="1:69">
+      <c r="BR8" s="2">
+        <v>-846.15</v>
+      </c>
+      <c r="BS8" s="2">
+        <v>-2380.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -17951,15 +18378,21 @@
       <c r="BQ9" s="13">
         <v>108.27</v>
       </c>
-    </row>
-    <row r="10" spans="1:69">
+      <c r="BR9" s="13">
+        <v>114.1</v>
+      </c>
+      <c r="BS9" s="13">
+        <v>110.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-1.1312616240474402E-3</v>
+        <v>-1.3650934643990315E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-117.76433506333852</v>
+        <v>-142.10622964393917</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -18197,39 +18630,47 @@
         <v>-3.8642664266426645</v>
       </c>
       <c r="BJ10" s="6">
-        <f>BJ6/BJ9</f>
+        <f t="shared" ref="BJ10:BS10" si="27">BJ6/BJ9</f>
         <v>-4.3436175011276505</v>
       </c>
       <c r="BK10" s="6">
-        <f>BK6/BK9</f>
+        <f t="shared" si="27"/>
         <v>9.5298737975465535</v>
       </c>
       <c r="BL10" s="6">
-        <f>BL6/BL9</f>
+        <f t="shared" si="27"/>
         <v>27.40094786729858</v>
       </c>
       <c r="BM10" s="6">
-        <f>BM6/BM9</f>
+        <f t="shared" si="27"/>
         <v>14.54637843424339</v>
       </c>
       <c r="BN10" s="6">
-        <f>BN6/BN9</f>
+        <f t="shared" si="27"/>
         <v>1.6750170998632012</v>
       </c>
       <c r="BO10" s="6">
-        <f>BO6/BO9</f>
+        <f t="shared" si="27"/>
         <v>-13.769860700717603</v>
       </c>
       <c r="BP10" s="6">
-        <f>BP6/BP9</f>
+        <f t="shared" si="27"/>
         <v>-37.028992093065526</v>
       </c>
       <c r="BQ10" s="6">
-        <f>BQ6/BQ9</f>
+        <f t="shared" si="27"/>
         <v>-24.540870047104463</v>
       </c>
-    </row>
-    <row r="11" spans="1:69">
+      <c r="BR10" s="6">
+        <f t="shared" si="27"/>
+        <v>-3.0035056967572307</v>
+      </c>
+      <c r="BS10" s="6">
+        <f t="shared" si="27"/>
+        <v>-21.338388883843432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -18499,8 +18940,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-11178.280000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:69">
+      <c r="BR11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-11520.980000000003</v>
+      </c>
+      <c r="BS11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-13870.550000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -18770,8 +19219,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>6050.0099999999957</v>
       </c>
-    </row>
-    <row r="13" spans="1:69">
+      <c r="BR12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>6553.4499999999953</v>
+      </c>
+      <c r="BS12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>6584.5499999999956</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -19041,19 +19498,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-17260.049999999985</v>
       </c>
-    </row>
-    <row r="14" spans="1:69">
+      <c r="BR13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-18106.199999999986</v>
+      </c>
+      <c r="BS13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-20486.869999999988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>94.920758428159616</v>
+        <v>97.606910230142617</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:71">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -19061,7 +19526,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:71">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -19269,10 +19734,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA49"/>
+  <dimension ref="A1:BC49"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="BA7" sqref="BA7"/>
+    <sheetView topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BC7" sqref="BC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19281,7 +19746,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:55">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -19289,7 +19754,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:55">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -19306,14 +19771,14 @@
         <v>9555800</v>
       </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:55">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:55">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -19467,8 +19932,14 @@
       <c r="BA4" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="BB4" s="6">
+        <v>51</v>
+      </c>
+      <c r="BC4" s="6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -19624,12 +20095,18 @@
       <c r="BA5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="BB5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-9860.6499999999833</v>
+        <v>-8561.6499999999833</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -19784,8 +20261,14 @@
       <c r="BA6" s="2">
         <v>-4112.42</v>
       </c>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="BB6" s="2">
+        <v>3964.54</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>-2665.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -19941,8 +20424,14 @@
       <c r="BA7" s="2">
         <v>-4236.21</v>
       </c>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="BB7" s="2">
+        <v>-4607.21</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>-1184.8599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -20098,8 +20587,14 @@
       <c r="BA8" s="2">
         <v>123.79</v>
       </c>
-    </row>
-    <row r="9" spans="1:53">
+      <c r="BB8" s="2">
+        <v>8571.74</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>-1480.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -20255,15 +20750,21 @@
       <c r="BA9" s="13">
         <v>6.83</v>
       </c>
-    </row>
-    <row r="10" spans="1:53">
+      <c r="BB9" s="13">
+        <v>7.05</v>
+      </c>
+      <c r="BC9" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-1.6093020422105046E-4</v>
+        <v>-1.4193078285189753E-4</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-1537.8168454955139</v>
+        <v>-1356.2621747761623</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -20468,8 +20969,16 @@
         <f t="shared" si="22"/>
         <v>-602.1112737920937</v>
       </c>
-    </row>
-    <row r="11" spans="1:53">
+      <c r="BB10" s="6">
+        <f t="shared" ref="BB10:BC10" si="23">BB6/BB9</f>
+        <v>562.3460992907801</v>
+      </c>
+      <c r="BC10" s="6">
+        <f t="shared" si="23"/>
+        <v>-380.79142857142858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -20675,8 +21184,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-9860.6499999999833</v>
       </c>
-    </row>
-    <row r="12" spans="1:53">
+      <c r="BB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-5896.1099999999833</v>
+      </c>
+      <c r="BC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-8561.6499999999833</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -20882,8 +21399,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>66575.26999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:53">
+      <c r="BB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>61968.05999999999</v>
+      </c>
+      <c r="BC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>60783.19999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -21089,19 +21614,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-76509.810000000027</v>
       </c>
-    </row>
-    <row r="14" spans="1:53">
+      <c r="BB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-67938.070000000022</v>
+      </c>
+      <c r="BC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-69418.760000000024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>6.4121094972286468</v>
+        <v>6.3126806595583185</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:53">
+    <row r="15" spans="1:55">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -21109,7 +21642,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:53">
+    <row r="16" spans="1:55">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -21317,10 +21850,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA49"/>
+  <dimension ref="A1:BC49"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="BA7" sqref="BA7"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BC7" sqref="BC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21329,7 +21862,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:55">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -21337,7 +21870,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:55">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -21354,14 +21887,14 @@
         <v>2209000</v>
       </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:55">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:55">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -21515,8 +22048,14 @@
       <c r="BA4" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="BB4" s="6">
+        <v>51</v>
+      </c>
+      <c r="BC4" s="6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -21672,12 +22211,18 @@
       <c r="BA5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="BB5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-89667.55</v>
+        <v>-84750.590000000011</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -21832,8 +22377,14 @@
       <c r="BA6" s="2">
         <v>-5945.81</v>
       </c>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="BB6" s="2">
+        <v>1937.65</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>2979.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -21989,8 +22540,14 @@
       <c r="BA7" s="2">
         <v>-7000.58</v>
       </c>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="BB7" s="2">
+        <v>713.93</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>-3901.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -22146,8 +22703,14 @@
       <c r="BA8" s="2">
         <v>1054.78</v>
       </c>
-    </row>
-    <row r="9" spans="1:53">
+      <c r="BB8" s="2">
+        <v>1223.73</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>6881.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -22303,15 +22866,21 @@
       <c r="BA9" s="13">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:53">
+      <c r="BB9" s="13">
+        <v>8.42</v>
+      </c>
+      <c r="BC9" s="13">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-4.7287141917403842E-3</v>
+        <v>-4.463015551675986E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-10445.729649554509</v>
+        <v>-9858.8013536522521</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -22516,8 +23085,16 @@
         <f t="shared" si="24"/>
         <v>-720.70424242424247</v>
       </c>
-    </row>
-    <row r="11" spans="1:53">
+      <c r="BB10" s="6">
+        <f t="shared" ref="BB10:BC10" si="25">BB6/BB9</f>
+        <v>230.12470308788599</v>
+      </c>
+      <c r="BC10" s="6">
+        <f t="shared" si="25"/>
+        <v>356.80359281437126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -22723,8 +23300,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-89667.55</v>
       </c>
-    </row>
-    <row r="12" spans="1:53">
+      <c r="BB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-87729.900000000009</v>
+      </c>
+      <c r="BC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-84750.590000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -22930,8 +23515,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-48662.079999999987</v>
       </c>
-    </row>
-    <row r="13" spans="1:53">
+      <c r="BB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-47948.149999999987</v>
+      </c>
+      <c r="BC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-51850.049999999988</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -23137,19 +23730,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-42112.919999999991</v>
       </c>
-    </row>
-    <row r="14" spans="1:53">
+      <c r="BB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-40889.189999999988</v>
+      </c>
+      <c r="BC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-34007.969999999987</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>8.5841346663441698</v>
+        <v>8.5964395629701631</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:53">
+    <row r="15" spans="1:55">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -23157,7 +23758,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:53">
+    <row r="16" spans="1:55">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -23365,10 +23966,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA49"/>
+  <dimension ref="A1:BC49"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BA7" sqref="BA7"/>
+    <sheetView topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BB9" sqref="BB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23377,7 +23978,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:55">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -23385,7 +23986,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:55">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -23402,14 +24003,14 @@
         <v>4010.0000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:55">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:55">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -23563,8 +24164,14 @@
       <c r="BA4" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="BB4" s="6">
+        <v>51</v>
+      </c>
+      <c r="BC4" s="6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -23720,12 +24327,18 @@
       <c r="BA5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="BB5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-58578.47</v>
+        <v>-60422.91</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -23880,8 +24493,14 @@
       <c r="BA6" s="2">
         <v>-3235.46</v>
       </c>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="BB6" s="2">
+        <v>31.84</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>-1876.28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -24037,8 +24656,14 @@
       <c r="BA7" s="2">
         <v>-1779.87</v>
       </c>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="BB7" s="2">
+        <v>331.84</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>-1356.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -24194,8 +24819,14 @@
       <c r="BA8" s="2">
         <v>-1455.59</v>
       </c>
-    </row>
-    <row r="9" spans="1:53">
+      <c r="BB8" s="2">
+        <v>-300</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>-519.69000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -24351,15 +24982,21 @@
       <c r="BA9" s="13">
         <v>137.13</v>
       </c>
-    </row>
-    <row r="10" spans="1:53">
+      <c r="BB9" s="13">
+        <v>139.02000000000001</v>
+      </c>
+      <c r="BC9" s="13">
+        <v>135.13999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-9.537789752863314E-2</v>
+        <v>-9.8783119569285302E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-382.46536908981892</v>
+        <v>-396.12030947283409</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -24564,8 +25201,16 @@
         <f t="shared" si="24"/>
         <v>-23.594107780937797</v>
       </c>
-    </row>
-    <row r="11" spans="1:53">
+      <c r="BB10" s="6">
+        <f t="shared" ref="BB10:BC10" si="25">BB6/BB9</f>
+        <v>0.22903179398647674</v>
+      </c>
+      <c r="BC10" s="6">
+        <f t="shared" si="25"/>
+        <v>-13.883972177001629</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -24771,8 +25416,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-58578.47</v>
       </c>
-    </row>
-    <row r="12" spans="1:53">
+      <c r="BB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-58546.630000000005</v>
+      </c>
+      <c r="BC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-60422.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -24978,8 +25631,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-32888.14</v>
       </c>
-    </row>
-    <row r="13" spans="1:53">
+      <c r="BB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-32556.3</v>
+      </c>
+      <c r="BC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-33912.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -25185,19 +25846,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-24424.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:53">
+      <c r="BB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-24724.3</v>
+      </c>
+      <c r="BC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-25243.989999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>153.16019366512452</v>
+        <v>152.53676359187992</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:53">
+    <row r="15" spans="1:55">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -25205,7 +25874,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:53">
+    <row r="16" spans="1:55">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -25413,10 +26082,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA49"/>
+  <dimension ref="A1:BC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="BA7" sqref="BA7"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BB9" sqref="BB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25425,7 +26094,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:55">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -25433,7 +26102,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:55">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -25450,14 +26119,14 @@
         <v>113800.00000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:55">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:55">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -25611,8 +26280,14 @@
       <c r="BA4" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="BB4" s="6">
+        <v>51</v>
+      </c>
+      <c r="BC4" s="6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -25768,12 +26443,18 @@
       <c r="BA5" s="5">
         <v>43250</v>
       </c>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="BB5" s="5">
+        <v>43251</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-135147.51999999999</v>
+        <v>-139029.32999999999</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -25928,8 +26609,14 @@
       <c r="BA6" s="2">
         <v>-6495.38</v>
       </c>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="BB6" s="2">
+        <v>-2135.65</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>-1746.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -26085,8 +26772,14 @@
       <c r="BA7" s="2">
         <v>-3385.08</v>
       </c>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="BB7" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>-449.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -26242,8 +26935,14 @@
       <c r="BA8" s="2">
         <v>-3110.29</v>
       </c>
-    </row>
-    <row r="9" spans="1:53">
+      <c r="BB8" s="2">
+        <v>-1135.6500000000001</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>-1296.46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -26399,15 +27098,21 @@
       <c r="BA9" s="13">
         <v>50.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:53">
+      <c r="BB9" s="13">
+        <v>51.15</v>
+      </c>
+      <c r="BC9" s="13">
+        <v>50.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-2.146044382242808E-2</v>
+        <v>-2.2128735976375397E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-2442.1985069923157</v>
+        <v>-2518.2501541115207</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -26612,8 +27317,16 @@
         <f t="shared" si="20"/>
         <v>-128.87658730158731</v>
       </c>
-    </row>
-    <row r="11" spans="1:53">
+      <c r="BB10" s="6">
+        <f t="shared" ref="BB10:BC10" si="21">BB6/BB9</f>
+        <v>-41.752688172043015</v>
+      </c>
+      <c r="BC10" s="6">
+        <f t="shared" si="21"/>
+        <v>-34.298958947161658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -26819,8 +27532,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-135147.51999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:53">
+      <c r="BB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-137283.16999999998</v>
+      </c>
+      <c r="BC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-139029.32999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -27026,8 +27747,16 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-154049.73000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:53">
+      <c r="BB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-155049.73000000004</v>
+      </c>
+      <c r="BC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-155499.43000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -27233,19 +27962,27 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>25722.979999999989</v>
       </c>
-    </row>
-    <row r="14" spans="1:53">
+      <c r="BB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>24587.329999999987</v>
+      </c>
+      <c r="BC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>23290.869999999988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>55.338466391268341</v>
+        <v>55.208705049817333</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:53">
+    <row r="15" spans="1:55">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -27253,7 +27990,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:53">
+    <row r="16" spans="1:55">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
update vip to latest
</commit_message>
<xml_diff>
--- a/stock_vip.xlsx
+++ b/stock_vip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunjim/Documents/stock_market/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81FDCBF-C9F5-5A46-9EC5-41F5F1D759F8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881B5D27-3841-834F-BFF0-DBB6BDE5843A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="1960" windowWidth="25600" windowHeight="16060" tabRatio="1000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="25">
   <si>
     <t>万元</t>
   </si>
@@ -1299,6 +1299,15 @@
                 <c:pt idx="4">
                   <c:v>6.81</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.89</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.95</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1785,6 +1794,15 @@
                 <c:pt idx="127">
                   <c:v>-75889.609999999957</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-72408.449999999953</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-79362.569999999949</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-91376.269999999946</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2191,6 +2209,15 @@
                 <c:pt idx="127">
                   <c:v>36224.640000000036</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>43603.250000000036</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>35758.790000000037</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>21320.590000000037</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2596,6 +2623,15 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>-119746.06999999993</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-123643.50999999994</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-122753.16999999994</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-120328.65999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3662,6 +3698,15 @@
                 <c:pt idx="127">
                   <c:v>-166516.47000000006</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-163525.96000000005</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-162960.79000000004</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-157759.34000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4068,6 +4113,15 @@
                 <c:pt idx="127">
                   <c:v>-48809.45</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-47120.81</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-45247.96</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-37702.080000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4473,6 +4527,15 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>-118817.95000000001</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-117516.07</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-118823.76000000001</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-121168.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4789,6 +4852,15 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>7.59</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.57</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5544,6 +5616,15 @@
                 <c:pt idx="127">
                   <c:v>65.760000000000005</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>66.2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>65.97</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>67.03</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6029,6 +6110,15 @@
                 <c:pt idx="127">
                   <c:v>-168586.33000000013</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-168608.42000000013</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-168881.15000000014</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-168950.72000000015</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6435,6 +6525,15 @@
                 <c:pt idx="127">
                   <c:v>-118324.5</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-118003.69</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-117812.83</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-118252.41</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6840,6 +6939,15 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>-48146.729999999989</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-48489.62999999999</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-48953.219999999987</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-48583.209999999985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7324,6 +7432,15 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>45.08</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>46.96</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>45.95</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>47.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9187,6 +9304,15 @@
                 <c:pt idx="127">
                   <c:v>-218991.13999999998</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-213921.05</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-213339.21</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-221417.69</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9593,6 +9719,15 @@
                 <c:pt idx="127">
                   <c:v>-204446.42</c:v>
                 </c:pt>
+                <c:pt idx="128">
+                  <c:v>-197628.11000000002</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-197577.42</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-204246.36000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9998,6 +10133,15 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>-12018.320000000011</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-13766.55000000001</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-13235.420000000011</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-14644.96000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10531,6 +10675,15 @@
                 <c:pt idx="143">
                   <c:v>36402.71</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>36574.86</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>36609.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>36720.449999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10985,6 +11138,15 @@
                 <c:pt idx="143">
                   <c:v>-876703.50999999966</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>-833974.49999999965</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-848710.84999999963</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>-825836.76999999967</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11438,6 +11600,15 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>913358.03999999957</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>870801.14999999956</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>885572.14999999956</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>862808.97999999952</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11739,6 +11910,15 @@
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>666.7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>681.42</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>678.55</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>700.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12606,6 +12786,15 @@
                 <c:pt idx="143">
                   <c:v>44.4</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>45.09</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>44.83</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>46.18</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13139,6 +13328,15 @@
                 <c:pt idx="143">
                   <c:v>-143190.45000000004</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>-141998.02000000005</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-142635.11000000004</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>-141696.52000000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13593,6 +13791,15 @@
                 <c:pt idx="143">
                   <c:v>-120546.40999999997</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>-119698.42999999998</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-120336.20999999998</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>-119455.64999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14046,6 +14253,15 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>-22598.029999999995</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>-22253.579999999994</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-22252.879999999994</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>-22194.839999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22210,10 +22426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:EQ49"/>
+  <dimension ref="A1:ET49"/>
   <sheetViews>
-    <sheetView topLeftCell="EG1" workbookViewId="0">
-      <selection activeCell="EQ7" sqref="EQ7"/>
+    <sheetView topLeftCell="EI1" workbookViewId="0">
+      <selection activeCell="ET7" sqref="ET7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22222,7 +22438,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:147">
+    <row r="1" spans="1:150">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -22230,7 +22446,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:147">
+    <row r="2" spans="1:150">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -22247,14 +22463,14 @@
         <v>125600</v>
       </c>
     </row>
-    <row r="3" spans="1:147">
+    <row r="3" spans="1:150">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:147">
+    <row r="4" spans="1:150">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -22690,8 +22906,17 @@
       <c r="EQ4" s="6">
         <v>144</v>
       </c>
+      <c r="ER4" s="6">
+        <v>145</v>
+      </c>
+      <c r="ES4" s="6">
+        <v>146</v>
+      </c>
+      <c r="ET4" s="6">
+        <v>147</v>
+      </c>
     </row>
-    <row r="5" spans="1:147">
+    <row r="5" spans="1:150">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -23129,12 +23354,21 @@
       <c r="EQ5" s="5">
         <v>43361</v>
       </c>
+      <c r="ER5" s="5">
+        <v>43362</v>
+      </c>
+      <c r="ES5" s="5">
+        <v>43363</v>
+      </c>
+      <c r="ET5" s="5">
+        <v>43364</v>
+      </c>
     </row>
-    <row r="6" spans="1:147">
+    <row r="6" spans="1:150">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>36402.71</v>
+        <v>36720.449999999997</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -23571,8 +23805,17 @@
       <c r="EQ6" s="2">
         <v>553.13</v>
       </c>
+      <c r="ER6" s="2">
+        <v>172.15</v>
+      </c>
+      <c r="ES6" s="2">
+        <v>34.64</v>
+      </c>
+      <c r="ET6" s="2">
+        <v>110.95</v>
+      </c>
     </row>
-    <row r="7" spans="1:147">
+    <row r="7" spans="1:150">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -24010,8 +24253,17 @@
       <c r="EQ7" s="2">
         <v>41004.15</v>
       </c>
+      <c r="ER7" s="2">
+        <v>42729.01</v>
+      </c>
+      <c r="ES7" s="2">
+        <v>-14736.35</v>
+      </c>
+      <c r="ET7" s="2">
+        <v>22874.080000000002</v>
+      </c>
     </row>
-    <row r="8" spans="1:147">
+    <row r="8" spans="1:150">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -24449,8 +24701,17 @@
       <c r="EQ8" s="2">
         <v>-40471.019999999997</v>
       </c>
+      <c r="ER8" s="2">
+        <v>-42556.89</v>
+      </c>
+      <c r="ES8" s="2">
+        <v>14771</v>
+      </c>
+      <c r="ET8" s="2">
+        <v>-22763.17</v>
+      </c>
     </row>
-    <row r="9" spans="1:147">
+    <row r="9" spans="1:150">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -24888,15 +25149,24 @@
       <c r="EQ9" s="13">
         <v>666.7</v>
       </c>
+      <c r="ER9" s="13">
+        <v>681.42</v>
+      </c>
+      <c r="ES9" s="13">
+        <v>678.55</v>
+      </c>
+      <c r="ET9" s="13">
+        <v>700.01</v>
+      </c>
     </row>
-    <row r="10" spans="1:147" s="9" customFormat="1">
+    <row r="10" spans="1:150" s="9" customFormat="1">
       <c r="A10" s="19">
         <f>B10/F2</f>
-        <v>4.102326669014566E-4</v>
+        <v>4.1391245968766673E-4</v>
       </c>
       <c r="B10" s="20">
         <f>SUM(D10:IX10)</f>
-        <v>51.525222962822951</v>
+        <v>51.987404936770943</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>3</v>
@@ -25454,31 +25724,43 @@
         <v>0.79413771712158809</v>
       </c>
       <c r="EL10" s="18">
-        <f>EL6/EL9</f>
+        <f t="shared" ref="EL10:ET10" si="67">EL6/EL9</f>
         <v>1.5773839009287927</v>
       </c>
       <c r="EM10" s="18">
-        <f>EM6/EM9</f>
+        <f t="shared" si="67"/>
         <v>0.5734285714285714</v>
       </c>
       <c r="EN10" s="18">
-        <f>EN6/EN9</f>
+        <f t="shared" si="67"/>
         <v>0.76032469381942458</v>
       </c>
       <c r="EO10" s="18">
-        <f>EO6/EO9</f>
+        <f t="shared" si="67"/>
         <v>2.1340177321511899</v>
       </c>
       <c r="EP10" s="18">
-        <f>EP6/EP9</f>
+        <f t="shared" si="67"/>
         <v>0.21030953376380052</v>
       </c>
       <c r="EQ10" s="18">
-        <f>EQ6/EQ9</f>
+        <f t="shared" si="67"/>
         <v>0.82965351732413373</v>
       </c>
+      <c r="ER10" s="18">
+        <f t="shared" si="67"/>
+        <v>0.25263420504241146</v>
+      </c>
+      <c r="ES10" s="18">
+        <f t="shared" si="67"/>
+        <v>5.1050033158941868E-2</v>
+      </c>
+      <c r="ET10" s="18">
+        <f t="shared" si="67"/>
+        <v>0.1584977357466322</v>
+      </c>
     </row>
-    <row r="11" spans="1:147">
+    <row r="11" spans="1:150">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -26060,8 +26342,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>36402.71</v>
       </c>
+      <c r="ER11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>36574.86</v>
+      </c>
+      <c r="ES11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>36609.5</v>
+      </c>
+      <c r="ET11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>36720.449999999997</v>
+      </c>
     </row>
-    <row r="12" spans="1:147">
+    <row r="12" spans="1:150">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -26643,8 +26937,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-876703.50999999966</v>
       </c>
+      <c r="ER12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-833974.49999999965</v>
+      </c>
+      <c r="ES12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-848710.84999999963</v>
+      </c>
+      <c r="ET12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-825836.76999999967</v>
+      </c>
     </row>
-    <row r="13" spans="1:147">
+    <row r="13" spans="1:150">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -27226,12 +27532,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>913358.03999999957</v>
       </c>
+      <c r="ER13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>870801.14999999956</v>
+      </c>
+      <c r="ES13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>885572.14999999956</v>
+      </c>
+      <c r="ET13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>862808.97999999952</v>
+      </c>
     </row>
-    <row r="14" spans="1:147">
+    <row r="14" spans="1:150">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>706.50271666491744</v>
+        <v>706.33358300266775</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -27241,7 +27559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:147">
+    <row r="15" spans="1:150">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -27249,7 +27567,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:147">
+    <row r="16" spans="1:150">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -27457,10 +27775,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:EQ49"/>
+  <dimension ref="A1:ET49"/>
   <sheetViews>
-    <sheetView topLeftCell="EB1" workbookViewId="0">
-      <selection activeCell="EQ7" sqref="EQ7"/>
+    <sheetView topLeftCell="EH1" workbookViewId="0">
+      <selection activeCell="ET7" sqref="ET7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -27469,7 +27787,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:147">
+    <row r="1" spans="1:150">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -27477,7 +27795,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:147">
+    <row r="2" spans="1:150">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -27494,14 +27812,14 @@
         <v>65400</v>
       </c>
     </row>
-    <row r="3" spans="1:147">
+    <row r="3" spans="1:150">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:147">
+    <row r="4" spans="1:150">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -27937,8 +28255,17 @@
       <c r="EQ4" s="6">
         <v>144</v>
       </c>
+      <c r="ER4" s="6">
+        <v>145</v>
+      </c>
+      <c r="ES4" s="6">
+        <v>146</v>
+      </c>
+      <c r="ET4" s="6">
+        <v>147</v>
+      </c>
     </row>
-    <row r="5" spans="1:147">
+    <row r="5" spans="1:150">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -28376,12 +28703,21 @@
       <c r="EQ5" s="5">
         <v>43361</v>
       </c>
+      <c r="ER5" s="5">
+        <v>43362</v>
+      </c>
+      <c r="ES5" s="5">
+        <v>43363</v>
+      </c>
+      <c r="ET5" s="5">
+        <v>43364</v>
+      </c>
     </row>
-    <row r="6" spans="1:147">
+    <row r="6" spans="1:150">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-143190.45000000004</v>
+        <v>-141696.52000000005</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -28818,8 +29154,17 @@
       <c r="EQ6" s="2">
         <v>197.51</v>
       </c>
+      <c r="ER6" s="2">
+        <v>1192.43</v>
+      </c>
+      <c r="ES6" s="2">
+        <v>-637.09</v>
+      </c>
+      <c r="ET6" s="2">
+        <v>938.59</v>
+      </c>
     </row>
-    <row r="7" spans="1:147">
+    <row r="7" spans="1:150">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -29257,8 +29602,17 @@
       <c r="EQ7" s="2">
         <v>710.53</v>
       </c>
+      <c r="ER7" s="2">
+        <v>847.98</v>
+      </c>
+      <c r="ES7" s="2">
+        <v>-637.78</v>
+      </c>
+      <c r="ET7" s="2">
+        <v>880.56</v>
+      </c>
     </row>
-    <row r="8" spans="1:147">
+    <row r="8" spans="1:150">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -29696,8 +30050,17 @@
       <c r="EQ8" s="2">
         <v>-513.02</v>
       </c>
+      <c r="ER8" s="2">
+        <v>344.45</v>
+      </c>
+      <c r="ES8" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="ET8" s="2">
+        <v>58.04</v>
+      </c>
     </row>
-    <row r="9" spans="1:147">
+    <row r="9" spans="1:150">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -30135,15 +30498,24 @@
       <c r="EQ9" s="13">
         <v>44.4</v>
       </c>
+      <c r="ER9" s="13">
+        <v>45.09</v>
+      </c>
+      <c r="ES9" s="13">
+        <v>44.83</v>
+      </c>
+      <c r="ET9" s="13">
+        <v>46.18</v>
+      </c>
     </row>
-    <row r="10" spans="1:147">
+    <row r="10" spans="1:150">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-3.982764996274054E-2</v>
+        <v>-3.9329807298216272E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-2604.7283075632313</v>
+        <v>-2572.1693973033443</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -30701,31 +31073,43 @@
         <v>0.52746275294640865</v>
       </c>
       <c r="EL10" s="6">
-        <f>EL6/EL9</f>
+        <f t="shared" ref="EL10:ET10" si="64">EL6/EL9</f>
         <v>-10.193141592920353</v>
       </c>
       <c r="EM10" s="6">
-        <f>EM6/EM9</f>
+        <f t="shared" si="64"/>
         <v>-9.9071863032214456</v>
       </c>
       <c r="EN10" s="6">
-        <f>EN6/EN9</f>
+        <f t="shared" si="64"/>
         <v>-6.4634856630824364</v>
       </c>
       <c r="EO10" s="6">
-        <f>EO6/EO9</f>
+        <f t="shared" si="64"/>
         <v>1.5404428377767738</v>
       </c>
       <c r="EP10" s="6">
-        <f>EP6/EP9</f>
+        <f t="shared" si="64"/>
         <v>-6.3390646492434666</v>
       </c>
       <c r="EQ10" s="6">
-        <f>EQ6/EQ9</f>
+        <f t="shared" si="64"/>
         <v>4.4484234234234235</v>
       </c>
+      <c r="ER10" s="6">
+        <f t="shared" si="64"/>
+        <v>26.445553337768906</v>
+      </c>
+      <c r="ES10" s="6">
+        <f t="shared" si="64"/>
+        <v>-14.211242471559226</v>
+      </c>
+      <c r="ET10" s="6">
+        <f t="shared" si="64"/>
+        <v>20.324599393676916</v>
+      </c>
     </row>
-    <row r="11" spans="1:147">
+    <row r="11" spans="1:150">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -31307,8 +31691,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-143190.45000000004</v>
       </c>
+      <c r="ER11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-141998.02000000005</v>
+      </c>
+      <c r="ES11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-142635.11000000004</v>
+      </c>
+      <c r="ET11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-141696.52000000005</v>
+      </c>
     </row>
-    <row r="12" spans="1:147">
+    <row r="12" spans="1:150">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -31890,8 +32286,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-120546.40999999997</v>
       </c>
+      <c r="ER12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-119698.42999999998</v>
+      </c>
+      <c r="ES12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-120336.20999999998</v>
+      </c>
+      <c r="ET12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-119455.64999999998</v>
+      </c>
     </row>
-    <row r="13" spans="1:147">
+    <row r="13" spans="1:150">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -32473,19 +32881,31 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-22598.029999999995</v>
       </c>
+      <c r="ER13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-22253.579999999994</v>
+      </c>
+      <c r="ES13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-22252.879999999994</v>
+      </c>
+      <c r="ET13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-22194.839999999993</v>
+      </c>
     </row>
-    <row r="14" spans="1:147">
+    <row r="14" spans="1:150">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>54.973276707679815</v>
+        <v>55.088331331736669</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:147">
+    <row r="15" spans="1:150">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -32493,7 +32913,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:147">
+    <row r="16" spans="1:150">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -32701,10 +33121,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:EQ49"/>
   <sheetViews>
     <sheetView topLeftCell="EF1" workbookViewId="0">
-      <selection activeCell="EQ7" sqref="EQ7"/>
+      <selection activeCell="EQ15" sqref="EQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -35945,27 +36368,27 @@
         <v>-25.293315143246932</v>
       </c>
       <c r="EL10" s="6">
-        <f>EL6/EL9</f>
+        <f t="shared" ref="EL10:EQ10" si="63">EL6/EL9</f>
         <v>13.103885480572597</v>
       </c>
       <c r="EM10" s="6">
-        <f>EM6/EM9</f>
+        <f t="shared" si="63"/>
         <v>-10.592148760330579</v>
       </c>
       <c r="EN10" s="6">
-        <f>EN6/EN9</f>
+        <f t="shared" si="63"/>
         <v>-6.643777412280703</v>
       </c>
       <c r="EO10" s="6">
-        <f>EO6/EO9</f>
+        <f t="shared" si="63"/>
         <v>33.465547823714012</v>
       </c>
       <c r="EP10" s="6">
-        <f>EP6/EP9</f>
+        <f t="shared" si="63"/>
         <v>-70.668278805120906</v>
       </c>
       <c r="EQ10" s="6">
-        <f>EQ6/EQ9</f>
+        <f t="shared" si="63"/>
         <v>-21.153922825003558</v>
       </c>
     </row>
@@ -37728,6 +38151,9 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
+      <c r="EQ14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:147">
       <c r="A15" s="6"/>
@@ -37945,10 +38371,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:EA49"/>
+  <dimension ref="A1:ED49"/>
   <sheetViews>
-    <sheetView topLeftCell="DK1" workbookViewId="0">
-      <selection activeCell="EA7" sqref="EA7"/>
+    <sheetView topLeftCell="DT1" workbookViewId="0">
+      <selection activeCell="ED7" sqref="ED7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -37957,7 +38383,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131">
+    <row r="1" spans="1:134">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -37965,7 +38391,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:131">
+    <row r="2" spans="1:134">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -37982,14 +38408,14 @@
         <v>9555800</v>
       </c>
     </row>
-    <row r="3" spans="1:131">
+    <row r="3" spans="1:134">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:131">
+    <row r="4" spans="1:134">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -38377,8 +38803,17 @@
       <c r="EA4" s="6">
         <v>128</v>
       </c>
+      <c r="EB4" s="6">
+        <v>129</v>
+      </c>
+      <c r="EC4" s="6">
+        <v>130</v>
+      </c>
+      <c r="ED4" s="6">
+        <v>131</v>
+      </c>
     </row>
-    <row r="5" spans="1:131">
+    <row r="5" spans="1:134">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -38768,12 +39203,21 @@
       <c r="EA5" s="5">
         <v>43361</v>
       </c>
+      <c r="EB5" s="5">
+        <v>43362</v>
+      </c>
+      <c r="EC5" s="5">
+        <v>43363</v>
+      </c>
+      <c r="ED5" s="5">
+        <v>43364</v>
+      </c>
     </row>
-    <row r="6" spans="1:131">
+    <row r="6" spans="1:134">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-75889.609999999957</v>
+        <v>-91376.269999999946</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -39162,8 +39606,17 @@
       <c r="EA6" s="2">
         <v>-1118.7</v>
       </c>
+      <c r="EB6" s="2">
+        <v>3481.16</v>
+      </c>
+      <c r="EC6" s="2">
+        <v>-6954.12</v>
+      </c>
+      <c r="ED6" s="2">
+        <v>-12013.7</v>
+      </c>
     </row>
-    <row r="7" spans="1:131">
+    <row r="7" spans="1:134">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -39553,8 +40006,17 @@
       <c r="EA7" s="2">
         <v>3256.54</v>
       </c>
+      <c r="EB7" s="2">
+        <v>7378.61</v>
+      </c>
+      <c r="EC7" s="2">
+        <v>-7844.46</v>
+      </c>
+      <c r="ED7" s="2">
+        <v>-14438.2</v>
+      </c>
     </row>
-    <row r="8" spans="1:131">
+    <row r="8" spans="1:134">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -39944,8 +40406,17 @@
       <c r="EA8" s="2">
         <v>-4375.24</v>
       </c>
+      <c r="EB8" s="2">
+        <v>-3897.44</v>
+      </c>
+      <c r="EC8" s="2">
+        <v>890.34</v>
+      </c>
+      <c r="ED8" s="2">
+        <v>2424.5100000000002</v>
+      </c>
     </row>
-    <row r="9" spans="1:131">
+    <row r="9" spans="1:134">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -40335,15 +40806,24 @@
       <c r="EA9" s="13">
         <v>6.81</v>
       </c>
+      <c r="EB9" s="13">
+        <v>6.93</v>
+      </c>
+      <c r="EC9" s="13">
+        <v>6.89</v>
+      </c>
+      <c r="ED9" s="13">
+        <v>6.95</v>
+      </c>
     </row>
-    <row r="10" spans="1:131">
+    <row r="10" spans="1:134">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-1.2503287607119927E-3</v>
+        <v>-1.4842771772396041E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-11947.891571611661</v>
+        <v>-14183.455850266208</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -40837,31 +41317,43 @@
         <v>-123.07440476190476</v>
       </c>
       <c r="DV10" s="6">
-        <f>DV6/DV9</f>
+        <f t="shared" ref="DV10:EB10" si="59">DV6/DV9</f>
         <v>155.51769911504425</v>
       </c>
       <c r="DW10" s="6">
-        <f>DW6/DW9</f>
+        <f t="shared" si="59"/>
         <v>1531.6375939849622</v>
       </c>
       <c r="DX10" s="6">
-        <f>DX6/DX9</f>
+        <f t="shared" si="59"/>
         <v>325.63250366032213</v>
       </c>
       <c r="DY10" s="6">
-        <f>DY6/DY9</f>
+        <f t="shared" si="59"/>
         <v>-349.30871491875928</v>
       </c>
       <c r="DZ10" s="6">
-        <f>DZ6/DZ9</f>
+        <f t="shared" si="59"/>
         <v>-558.75111773472429</v>
       </c>
       <c r="EA10" s="6">
-        <f>EA6/EA9</f>
+        <f t="shared" si="59"/>
         <v>-164.27312775330398</v>
       </c>
+      <c r="EB10" s="6">
+        <f t="shared" si="59"/>
+        <v>502.33189033189035</v>
+      </c>
+      <c r="EC10" s="6">
+        <f>EC6/EC9</f>
+        <v>-1009.3062409288825</v>
+      </c>
+      <c r="ED10" s="6">
+        <f>ED6/ED9</f>
+        <v>-1728.5899280575541</v>
+      </c>
     </row>
-    <row r="11" spans="1:131">
+    <row r="11" spans="1:134">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -41379,8 +41871,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-75889.609999999957</v>
       </c>
+      <c r="EB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-72408.449999999953</v>
+      </c>
+      <c r="EC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-79362.569999999949</v>
+      </c>
+      <c r="ED11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-91376.269999999946</v>
+      </c>
     </row>
-    <row r="12" spans="1:131">
+    <row r="12" spans="1:134">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -41898,8 +42402,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>36224.640000000036</v>
       </c>
+      <c r="EB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>43603.250000000036</v>
+      </c>
+      <c r="EC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>35758.790000000037</v>
+      </c>
+      <c r="ED12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>21320.590000000037</v>
+      </c>
     </row>
-    <row r="13" spans="1:131">
+    <row r="13" spans="1:134">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -42417,12 +42933,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-119746.06999999993</v>
       </c>
+      <c r="EB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-123643.50999999994</v>
+      </c>
+      <c r="EC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-122753.16999999994</v>
+      </c>
+      <c r="ED13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-120328.65999999995</v>
+      </c>
     </row>
-    <row r="14" spans="1:131">
+    <row r="14" spans="1:134">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>6.3517156600512354</v>
+        <v>6.4424545727538547</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -42435,7 +42963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:131">
+    <row r="15" spans="1:134">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -42443,7 +42971,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:131">
+    <row r="16" spans="1:134">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -42651,10 +43179,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:EA49"/>
+  <dimension ref="A1:ED49"/>
   <sheetViews>
-    <sheetView topLeftCell="DL1" workbookViewId="0">
-      <selection activeCell="EA7" sqref="EA7"/>
+    <sheetView topLeftCell="DT1" workbookViewId="0">
+      <selection activeCell="ED7" sqref="ED7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -42663,7 +43191,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131">
+    <row r="1" spans="1:134">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -42671,7 +43199,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:131">
+    <row r="2" spans="1:134">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -42688,14 +43216,14 @@
         <v>2209000</v>
       </c>
     </row>
-    <row r="3" spans="1:131">
+    <row r="3" spans="1:134">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:131">
+    <row r="4" spans="1:134">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -43083,8 +43611,17 @@
       <c r="EA4" s="6">
         <v>128</v>
       </c>
+      <c r="EB4" s="6">
+        <v>129</v>
+      </c>
+      <c r="EC4" s="6">
+        <v>130</v>
+      </c>
+      <c r="ED4" s="6">
+        <v>131</v>
+      </c>
     </row>
-    <row r="5" spans="1:131">
+    <row r="5" spans="1:134">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -43474,12 +44011,21 @@
       <c r="EA5" s="5">
         <v>43361</v>
       </c>
+      <c r="EB5" s="5">
+        <v>43362</v>
+      </c>
+      <c r="EC5" s="5">
+        <v>43363</v>
+      </c>
+      <c r="ED5" s="5">
+        <v>43364</v>
+      </c>
     </row>
-    <row r="6" spans="1:131">
+    <row r="6" spans="1:134">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-166516.47000000006</v>
+        <v>-157759.34000000003</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -43868,8 +44414,17 @@
       <c r="EA6" s="2">
         <v>4902.72</v>
       </c>
+      <c r="EB6" s="2">
+        <v>2990.51</v>
+      </c>
+      <c r="EC6" s="2">
+        <v>565.16999999999996</v>
+      </c>
+      <c r="ED6" s="2">
+        <v>5201.45</v>
+      </c>
     </row>
-    <row r="7" spans="1:131">
+    <row r="7" spans="1:134">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -44259,8 +44814,17 @@
       <c r="EA7" s="2">
         <v>5093.88</v>
       </c>
+      <c r="EB7" s="2">
+        <v>1688.64</v>
+      </c>
+      <c r="EC7" s="2">
+        <v>1872.85</v>
+      </c>
+      <c r="ED7" s="2">
+        <v>7545.88</v>
+      </c>
     </row>
-    <row r="8" spans="1:131">
+    <row r="8" spans="1:134">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -44650,8 +45214,17 @@
       <c r="EA8" s="2">
         <v>-191.16</v>
       </c>
+      <c r="EB8" s="2">
+        <v>1301.8800000000001</v>
+      </c>
+      <c r="EC8" s="2">
+        <v>-1307.69</v>
+      </c>
+      <c r="ED8" s="2">
+        <v>-2344.4299999999998</v>
+      </c>
     </row>
-    <row r="9" spans="1:131">
+    <row r="9" spans="1:134">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -45041,15 +45614,24 @@
       <c r="EA9" s="13">
         <v>7.59</v>
       </c>
+      <c r="EB9" s="13">
+        <v>7.57</v>
+      </c>
+      <c r="EC9" s="13">
+        <v>7.7</v>
+      </c>
+      <c r="ED9" s="13">
+        <v>7.95</v>
+      </c>
     </row>
-    <row r="10" spans="1:131">
+    <row r="10" spans="1:134">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-9.4205863947326857E-3</v>
+        <v>-8.9123398136131994E-3</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-20810.075345964502</v>
+        <v>-19687.358648271558</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -45543,31 +46125,43 @@
         <v>-201.12220762155059</v>
       </c>
       <c r="DV10" s="6">
-        <f>DV6/DV9</f>
+        <f t="shared" ref="DV10:ED10" si="61">DV6/DV9</f>
         <v>-1612.8549511854951</v>
       </c>
       <c r="DW10" s="6">
-        <f>DW6/DW9</f>
+        <f t="shared" si="61"/>
         <v>47.787500000000001</v>
       </c>
       <c r="DX10" s="6">
-        <f>DX6/DX9</f>
+        <f t="shared" si="61"/>
         <v>-276.51657458563534</v>
       </c>
       <c r="DY10" s="6">
-        <f>DY6/DY9</f>
+        <f t="shared" si="61"/>
         <v>104.36376021798365</v>
       </c>
       <c r="DZ10" s="6">
-        <f>DZ6/DZ9</f>
+        <f t="shared" si="61"/>
         <v>-122.05117565698477</v>
       </c>
       <c r="EA10" s="6">
-        <f>EA6/EA9</f>
+        <f t="shared" si="61"/>
         <v>645.94466403162062</v>
       </c>
+      <c r="EB10" s="6">
+        <f t="shared" si="61"/>
+        <v>395.04755614266844</v>
+      </c>
+      <c r="EC10" s="6">
+        <f t="shared" si="61"/>
+        <v>73.398701298701297</v>
+      </c>
+      <c r="ED10" s="6">
+        <f t="shared" si="61"/>
+        <v>654.27044025157227</v>
+      </c>
     </row>
-    <row r="11" spans="1:131">
+    <row r="11" spans="1:134">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -46085,8 +46679,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-166516.47000000006</v>
       </c>
+      <c r="EB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-163525.96000000005</v>
+      </c>
+      <c r="EC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-162960.79000000004</v>
+      </c>
+      <c r="ED11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-157759.34000000003</v>
+      </c>
     </row>
-    <row r="12" spans="1:131">
+    <row r="12" spans="1:134">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -46604,8 +47210,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-48809.45</v>
       </c>
+      <c r="EB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-47120.81</v>
+      </c>
+      <c r="EC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-45247.96</v>
+      </c>
+      <c r="ED12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-37702.080000000002</v>
+      </c>
     </row>
-    <row r="13" spans="1:131">
+    <row r="13" spans="1:134">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -47123,12 +47741,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-118817.95000000001</v>
       </c>
+      <c r="EB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-117516.07</v>
+      </c>
+      <c r="EC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-118823.76000000001</v>
+      </c>
+      <c r="ED13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-121168.19</v>
+      </c>
     </row>
-    <row r="14" spans="1:131">
+    <row r="14" spans="1:134">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>8.0017235512936757</v>
+        <v>8.0132303585504303</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -47138,7 +47768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:131">
+    <row r="15" spans="1:134">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -47146,7 +47776,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:131">
+    <row r="16" spans="1:134">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -47354,10 +47984,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:EA49"/>
+  <dimension ref="A1:ED49"/>
   <sheetViews>
-    <sheetView topLeftCell="DL2" workbookViewId="0">
-      <selection activeCell="EA7" sqref="EA7"/>
+    <sheetView topLeftCell="DU1" workbookViewId="0">
+      <selection activeCell="ED7" sqref="ED7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -47366,7 +47996,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131">
+    <row r="1" spans="1:134">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -47374,7 +48004,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:131">
+    <row r="2" spans="1:134">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -47391,14 +48021,14 @@
         <v>4010.0000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:131">
+    <row r="3" spans="1:134">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:131">
+    <row r="4" spans="1:134">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -47786,8 +48416,17 @@
       <c r="EA4" s="6">
         <v>128</v>
       </c>
+      <c r="EB4" s="6">
+        <v>129</v>
+      </c>
+      <c r="EC4" s="6">
+        <v>130</v>
+      </c>
+      <c r="ED4" s="6">
+        <v>131</v>
+      </c>
     </row>
-    <row r="5" spans="1:131">
+    <row r="5" spans="1:134">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -48177,12 +48816,21 @@
       <c r="EA5" s="5">
         <v>43361</v>
       </c>
+      <c r="EB5" s="5">
+        <v>43362</v>
+      </c>
+      <c r="EC5" s="5">
+        <v>43363</v>
+      </c>
+      <c r="ED5" s="5">
+        <v>43364</v>
+      </c>
     </row>
-    <row r="6" spans="1:131">
+    <row r="6" spans="1:134">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-168586.33000000013</v>
+        <v>-168950.72000000015</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -48571,8 +49219,17 @@
       <c r="EA6" s="2">
         <v>-754.57</v>
       </c>
+      <c r="EB6" s="2">
+        <v>-22.09</v>
+      </c>
+      <c r="EC6" s="2">
+        <v>-272.73</v>
+      </c>
+      <c r="ED6" s="2">
+        <v>-69.569999999999993</v>
+      </c>
     </row>
-    <row r="7" spans="1:131">
+    <row r="7" spans="1:134">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -48962,8 +49619,17 @@
       <c r="EA7" s="2">
         <v>-83.83</v>
       </c>
+      <c r="EB7" s="2">
+        <v>320.81</v>
+      </c>
+      <c r="EC7" s="2">
+        <v>190.86</v>
+      </c>
+      <c r="ED7" s="2">
+        <v>-439.58</v>
+      </c>
     </row>
-    <row r="8" spans="1:131">
+    <row r="8" spans="1:134">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -49353,8 +50019,17 @@
       <c r="EA8" s="2">
         <v>-670.74</v>
       </c>
+      <c r="EB8" s="2">
+        <v>-342.9</v>
+      </c>
+      <c r="EC8" s="2">
+        <v>-463.59</v>
+      </c>
+      <c r="ED8" s="2">
+        <v>370.01</v>
+      </c>
     </row>
-    <row r="9" spans="1:131">
+    <row r="9" spans="1:134">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -49744,15 +50419,24 @@
       <c r="EA9" s="13">
         <v>65.760000000000005</v>
       </c>
+      <c r="EB9" s="13">
+        <v>66.2</v>
+      </c>
+      <c r="EC9" s="13">
+        <v>65.97</v>
+      </c>
+      <c r="ED9" s="13">
+        <v>67.03</v>
+      </c>
     </row>
-    <row r="10" spans="1:131">
+    <row r="10" spans="1:134">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-0.43519690354433893</v>
+        <v>-0.43656990383569966</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-1745.1395832127994</v>
+        <v>-1750.6453143811559</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -50246,31 +50930,43 @@
         <v>-15.914084507042254</v>
       </c>
       <c r="DV10" s="6">
-        <f>DV6/DV9</f>
+        <f t="shared" ref="DV10:ED10" si="61">DV6/DV9</f>
         <v>-5.9307541351275583</v>
       </c>
       <c r="DW10" s="6">
-        <f>DW6/DW9</f>
+        <f t="shared" si="61"/>
         <v>22.194965986394557</v>
       </c>
       <c r="DX10" s="6">
-        <f>DX6/DX9</f>
+        <f t="shared" si="61"/>
         <v>-8.1086603518267921</v>
       </c>
       <c r="DY10" s="6">
-        <f>DY6/DY9</f>
+        <f t="shared" si="61"/>
         <v>-43.966021445481125</v>
       </c>
       <c r="DZ10" s="6">
-        <f>DZ6/DZ9</f>
+        <f t="shared" si="61"/>
         <v>-59.01216507545427</v>
       </c>
       <c r="EA10" s="6">
-        <f>EA6/EA9</f>
+        <f t="shared" si="61"/>
         <v>-11.474604622871047</v>
       </c>
+      <c r="EB10" s="6">
+        <f t="shared" si="61"/>
+        <v>-0.33368580060422959</v>
+      </c>
+      <c r="EC10" s="6">
+        <f t="shared" si="61"/>
+        <v>-4.1341518872214644</v>
+      </c>
+      <c r="ED10" s="6">
+        <f t="shared" si="61"/>
+        <v>-1.0378934805311053</v>
+      </c>
     </row>
-    <row r="11" spans="1:131">
+    <row r="11" spans="1:134">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -50788,8 +51484,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-168586.33000000013</v>
       </c>
+      <c r="EB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-168608.42000000013</v>
+      </c>
+      <c r="EC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-168881.15000000014</v>
+      </c>
+      <c r="ED11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-168950.72000000015</v>
+      </c>
     </row>
-    <row r="12" spans="1:131">
+    <row r="12" spans="1:134">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -51307,8 +52015,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-118324.5</v>
       </c>
+      <c r="EB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-118003.69</v>
+      </c>
+      <c r="EC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-117812.83</v>
+      </c>
+      <c r="ED12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-118252.41</v>
+      </c>
     </row>
-    <row r="13" spans="1:131">
+    <row r="13" spans="1:134">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -51826,12 +52546,24 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-48146.729999999989</v>
       </c>
+      <c r="EB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-48489.62999999999</v>
+      </c>
+      <c r="EC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-48953.219999999987</v>
+      </c>
+      <c r="ED13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-48583.209999999985</v>
+      </c>
     </row>
-    <row r="14" spans="1:131">
+    <row r="14" spans="1:134">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>96.60335002523577</v>
+        <v>96.507681260223379</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -51844,7 +52576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:131">
+    <row r="15" spans="1:134">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -51852,7 +52584,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:131">
+    <row r="16" spans="1:134">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -52060,10 +52792,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:EA49"/>
+  <dimension ref="A1:ED49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DO1" workbookViewId="0">
-      <selection activeCell="EA7" sqref="EA7"/>
+    <sheetView tabSelected="1" topLeftCell="DT1" workbookViewId="0">
+      <selection activeCell="ED7" sqref="ED7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -52072,7 +52804,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131">
+    <row r="1" spans="1:134">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -52080,7 +52812,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:131">
+    <row r="2" spans="1:134">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
@@ -52097,14 +52829,14 @@
         <v>113800.00000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:131">
+    <row r="3" spans="1:134">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:131">
+    <row r="4" spans="1:134">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -52492,8 +53224,17 @@
       <c r="EA4" s="6">
         <v>128</v>
       </c>
+      <c r="EB4" s="6">
+        <v>129</v>
+      </c>
+      <c r="EC4" s="6">
+        <v>130</v>
+      </c>
+      <c r="ED4" s="6">
+        <v>131</v>
+      </c>
     </row>
-    <row r="5" spans="1:131">
+    <row r="5" spans="1:134">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -52883,12 +53624,21 @@
       <c r="EA5" s="5">
         <v>43361</v>
       </c>
+      <c r="EB5" s="5">
+        <v>43362</v>
+      </c>
+      <c r="EC5" s="5">
+        <v>43363</v>
+      </c>
+      <c r="ED5" s="5">
+        <v>43364</v>
+      </c>
     </row>
-    <row r="6" spans="1:131">
+    <row r="6" spans="1:134">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
         <f>SUM(D6:IX6)</f>
-        <v>-218991.13999999998</v>
+        <v>-221417.69</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>1</v>
@@ -53277,8 +54027,17 @@
       <c r="EA6" s="2">
         <v>712.93</v>
       </c>
+      <c r="EB6" s="2">
+        <v>5070.09</v>
+      </c>
+      <c r="EC6" s="2">
+        <v>581.84</v>
+      </c>
+      <c r="ED6" s="2">
+        <v>-8078.48</v>
+      </c>
     </row>
-    <row r="7" spans="1:131">
+    <row r="7" spans="1:134">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
@@ -53668,8 +54427,17 @@
       <c r="EA7" s="2">
         <v>-238.87</v>
       </c>
+      <c r="EB7" s="2">
+        <v>6818.31</v>
+      </c>
+      <c r="EC7" s="2">
+        <v>50.69</v>
+      </c>
+      <c r="ED7" s="2">
+        <v>-6668.94</v>
+      </c>
     </row>
-    <row r="8" spans="1:131">
+    <row r="8" spans="1:134">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
@@ -54059,8 +54827,17 @@
       <c r="EA8" s="2">
         <v>951.79</v>
       </c>
+      <c r="EB8" s="2">
+        <v>-1748.23</v>
+      </c>
+      <c r="EC8" s="2">
+        <v>531.13</v>
+      </c>
+      <c r="ED8" s="2">
+        <v>-1409.54</v>
+      </c>
     </row>
-    <row r="9" spans="1:131">
+    <row r="9" spans="1:134">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8" t="s">
@@ -54450,15 +55227,24 @@
       <c r="EA9" s="13">
         <v>45.08</v>
       </c>
+      <c r="EB9" s="13">
+        <v>46.96</v>
+      </c>
+      <c r="EC9" s="13">
+        <v>45.95</v>
+      </c>
+      <c r="ED9" s="13">
+        <v>47.01</v>
+      </c>
     </row>
-    <row r="10" spans="1:131">
+    <row r="10" spans="1:134">
       <c r="A10" s="4">
         <f>B10/F2</f>
-        <v>-3.8096353477872616E-2</v>
+        <v>-3.854641841304958E-2</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(D10:IX10)</f>
-        <v>-4335.3650257819045</v>
+        <v>-4386.5824154050424</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
@@ -54952,31 +55738,43 @@
         <v>-38.356578001437818</v>
       </c>
       <c r="DV10" s="6">
-        <f>DV6/DV9</f>
+        <f t="shared" ref="DV10:ED10" si="57">DV6/DV9</f>
         <v>-22.948458574181117</v>
       </c>
       <c r="DW10" s="6">
-        <f>DW6/DW9</f>
+        <f t="shared" si="57"/>
         <v>34.394862036156042</v>
       </c>
       <c r="DX10" s="6">
-        <f>DX6/DX9</f>
+        <f t="shared" si="57"/>
         <v>11.454566635601118</v>
       </c>
       <c r="DY10" s="6">
-        <f>DY6/DY9</f>
+        <f t="shared" si="57"/>
         <v>92.262218254853835</v>
       </c>
       <c r="DZ10" s="6">
-        <f>DZ6/DZ9</f>
+        <f t="shared" si="57"/>
         <v>-16.528230305735327</v>
       </c>
       <c r="EA10" s="6">
-        <f>EA6/EA9</f>
+        <f t="shared" si="57"/>
         <v>15.814773735581188</v>
       </c>
+      <c r="EB10" s="6">
+        <f t="shared" si="57"/>
+        <v>107.96614139693357</v>
+      </c>
+      <c r="EC10" s="6">
+        <f t="shared" si="57"/>
+        <v>12.662459194776931</v>
+      </c>
+      <c r="ED10" s="6">
+        <f t="shared" si="57"/>
+        <v>-171.84599021484792</v>
+      </c>
     </row>
-    <row r="11" spans="1:131">
+    <row r="11" spans="1:134">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
@@ -55494,8 +56292,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
         <v>-218991.13999999998</v>
       </c>
+      <c r="EB11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-213921.05</v>
+      </c>
+      <c r="EC11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-213339.21</v>
+      </c>
+      <c r="ED11" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(6, 4)) : INDIRECT(ADDRESS(6, COLUMN())))</f>
+        <v>-221417.69</v>
+      </c>
     </row>
-    <row r="12" spans="1:131">
+    <row r="12" spans="1:134">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
@@ -56013,8 +56823,20 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
         <v>-204446.42</v>
       </c>
+      <c r="EB12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-197628.11000000002</v>
+      </c>
+      <c r="EC12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-197577.42</v>
+      </c>
+      <c r="ED12" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(7, 4)) : INDIRECT(ADDRESS(7, COLUMN())))</f>
+        <v>-204246.36000000002</v>
+      </c>
     </row>
-    <row r="13" spans="1:131">
+    <row r="13" spans="1:134">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8" t="s">
@@ -56532,19 +57354,31 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
         <v>-12018.320000000011</v>
       </c>
+      <c r="EB13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-13766.55000000001</v>
+      </c>
+      <c r="EC13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-13235.420000000011</v>
+      </c>
+      <c r="ED13" s="12">
+        <f ca="1">SUM(INDIRECT(ADDRESS(8, 4)) : INDIRECT(ADDRESS(8, COLUMN())))</f>
+        <v>-14644.96000000001</v>
+      </c>
     </row>
-    <row r="14" spans="1:131">
+    <row r="14" spans="1:134">
       <c r="A14" s="6"/>
       <c r="B14" s="6">
         <f>B6/B10</f>
-        <v>50.512733921523449</v>
+        <v>50.476126750158194</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:131">
+    <row r="15" spans="1:134">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -56552,7 +57386,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:131">
+    <row r="16" spans="1:134">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>

</xml_diff>